<commit_message>
all stations entered. need coords
</commit_message>
<xml_diff>
--- a/Data/noaa_temp_precip_elevation/Central America/PuertoRico_2015/PuertoRico_2015.xlsx
+++ b/Data/noaa_temp_precip_elevation/Central America/PuertoRico_2015/PuertoRico_2015.xlsx
@@ -426,8 +426,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:S196"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A169" workbookViewId="0">
-      <selection activeCell="F190" sqref="F190"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C187" sqref="C187"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>

</xml_diff>

<commit_message>
convert to C and mm
</commit_message>
<xml_diff>
--- a/Data/noaa_temp_precip_elevation/Central America/PuertoRico_2015/PuertoRico_2015.xlsx
+++ b/Data/noaa_temp_precip_elevation/Central America/PuertoRico_2015/PuertoRico_2015.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="20225"/>
-  <workbookPr autoCompressPictures="0"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+  <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="40" windowWidth="24060" windowHeight="15560"/>
+    <workbookView xWindow="384" yWindow="36" windowWidth="24060" windowHeight="14292"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="24">
   <si>
     <t>Station</t>
   </si>
@@ -88,15 +88,21 @@
   <si>
     <t>TOA BAJA LEVITOWN</t>
   </si>
+  <si>
+    <t>Temp ( C)</t>
+  </si>
+  <si>
+    <t>Rainfall (mm)</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="0.000000"/>
+    <numFmt numFmtId="164" formatCode="0.000000"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -160,8 +166,8 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -463,24 +469,25 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S196"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:U196"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="D142" sqref="D142"/>
+    <sheetView tabSelected="1" topLeftCell="D167" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="H181" sqref="H181"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="25.1640625" customWidth="1"/>
-    <col min="2" max="2" width="11.83203125" customWidth="1"/>
+    <col min="1" max="1" width="25.109375" customWidth="1"/>
+    <col min="2" max="2" width="11.77734375" customWidth="1"/>
     <col min="3" max="3" width="13" customWidth="1"/>
     <col min="4" max="4" width="15.6640625" customWidth="1"/>
-    <col min="6" max="6" width="26.1640625" customWidth="1"/>
-    <col min="7" max="7" width="28.1640625" customWidth="1"/>
+    <col min="6" max="6" width="16.5546875" customWidth="1"/>
+    <col min="7" max="8" width="12.109375" customWidth="1"/>
+    <col min="9" max="9" width="28.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" ht="18">
+    <row r="1" spans="1:21" ht="18">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -497,13 +504,19 @@
         <v>4</v>
       </c>
       <c r="F1" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="G1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="H1" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="I1" s="2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:19">
+    <row r="2" spans="1:21">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -519,14 +532,22 @@
       <c r="E2">
         <v>201501</v>
       </c>
-      <c r="F2" s="1">
+      <c r="F2">
+        <f>(G2-32)*5/9</f>
+        <v>26.055555555555557</v>
+      </c>
+      <c r="G2" s="1">
         <v>78.900000000000006</v>
       </c>
-      <c r="G2">
+      <c r="H2" s="1">
+        <f>I2*25.4</f>
+        <v>125.98399999999999</v>
+      </c>
+      <c r="I2">
         <v>4.96</v>
       </c>
     </row>
-    <row r="3" spans="1:19">
+    <row r="3" spans="1:21">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -542,14 +563,22 @@
       <c r="E3">
         <v>201502</v>
       </c>
-      <c r="F3" s="1">
+      <c r="F3">
+        <f t="shared" ref="F3:F66" si="0">(G3-32)*5/9</f>
+        <v>26.166666666666664</v>
+      </c>
+      <c r="G3" s="1">
         <v>79.099999999999994</v>
       </c>
-      <c r="G3">
+      <c r="H3" s="1">
+        <f t="shared" ref="H3:H66" si="1">I3*25.4</f>
+        <v>83.057999999999993</v>
+      </c>
+      <c r="I3">
         <v>3.27</v>
       </c>
     </row>
-    <row r="4" spans="1:19">
+    <row r="4" spans="1:21">
       <c r="A4" t="s">
         <v>1</v>
       </c>
@@ -565,14 +594,22 @@
       <c r="E4">
         <v>201503</v>
       </c>
-      <c r="F4" s="1">
+      <c r="F4">
+        <f t="shared" si="0"/>
+        <v>25.944444444444443</v>
+      </c>
+      <c r="G4" s="1">
         <v>78.7</v>
       </c>
-      <c r="G4">
+      <c r="H4" s="1">
+        <f t="shared" si="1"/>
+        <v>38.099999999999994</v>
+      </c>
+      <c r="I4">
         <v>1.5</v>
       </c>
     </row>
-    <row r="5" spans="1:19">
+    <row r="5" spans="1:21">
       <c r="A5" t="s">
         <v>1</v>
       </c>
@@ -588,14 +625,22 @@
       <c r="E5">
         <v>201504</v>
       </c>
-      <c r="F5" s="1">
+      <c r="F5">
+        <f t="shared" si="0"/>
+        <v>27.5</v>
+      </c>
+      <c r="G5" s="1">
         <v>81.5</v>
       </c>
-      <c r="G5">
+      <c r="H5" s="1">
+        <f t="shared" si="1"/>
+        <v>35.051999999999992</v>
+      </c>
+      <c r="I5">
         <v>1.38</v>
       </c>
     </row>
-    <row r="6" spans="1:19">
+    <row r="6" spans="1:21">
       <c r="A6" t="s">
         <v>1</v>
       </c>
@@ -611,14 +656,22 @@
       <c r="E6">
         <v>201505</v>
       </c>
-      <c r="F6" s="1">
+      <c r="F6">
+        <f t="shared" si="0"/>
+        <v>28.388888888888886</v>
+      </c>
+      <c r="G6" s="1">
         <v>83.1</v>
       </c>
-      <c r="G6">
+      <c r="H6" s="1">
+        <f t="shared" si="1"/>
+        <v>57.911999999999992</v>
+      </c>
+      <c r="I6">
         <v>2.2799999999999998</v>
       </c>
     </row>
-    <row r="7" spans="1:19">
+    <row r="7" spans="1:21">
       <c r="A7" t="s">
         <v>1</v>
       </c>
@@ -634,14 +687,22 @@
       <c r="E7">
         <v>201506</v>
       </c>
-      <c r="F7" s="1">
+      <c r="F7">
+        <f t="shared" si="0"/>
+        <v>28.833333333333332</v>
+      </c>
+      <c r="G7" s="1">
         <v>83.9</v>
       </c>
-      <c r="G7">
+      <c r="H7" s="1">
+        <f t="shared" si="1"/>
+        <v>53.593999999999994</v>
+      </c>
+      <c r="I7">
         <v>2.11</v>
       </c>
     </row>
-    <row r="8" spans="1:19">
+    <row r="8" spans="1:21">
       <c r="A8" t="s">
         <v>1</v>
       </c>
@@ -657,14 +718,22 @@
       <c r="E8">
         <v>201507</v>
       </c>
-      <c r="F8" s="1">
+      <c r="F8">
+        <f t="shared" si="0"/>
+        <v>28.722222222222221</v>
+      </c>
+      <c r="G8" s="1">
         <v>83.7</v>
       </c>
-      <c r="G8">
+      <c r="H8" s="1">
+        <f t="shared" si="1"/>
+        <v>40.893999999999998</v>
+      </c>
+      <c r="I8">
         <v>1.61</v>
       </c>
     </row>
-    <row r="9" spans="1:19">
+    <row r="9" spans="1:21">
       <c r="A9" t="s">
         <v>1</v>
       </c>
@@ -680,14 +749,22 @@
       <c r="E9">
         <v>201508</v>
       </c>
-      <c r="F9" s="1">
+      <c r="F9">
+        <f t="shared" si="0"/>
+        <v>28.444444444444443</v>
+      </c>
+      <c r="G9" s="1">
         <v>83.2</v>
       </c>
-      <c r="G9">
+      <c r="H9" s="1">
+        <f t="shared" si="1"/>
+        <v>150.62199999999999</v>
+      </c>
+      <c r="I9">
         <v>5.93</v>
       </c>
     </row>
-    <row r="10" spans="1:19">
+    <row r="10" spans="1:21">
       <c r="A10" t="s">
         <v>1</v>
       </c>
@@ -703,14 +780,22 @@
       <c r="E10">
         <v>201509</v>
       </c>
-      <c r="F10" s="1">
+      <c r="F10">
+        <f t="shared" si="0"/>
+        <v>29.055555555555557</v>
+      </c>
+      <c r="G10" s="1">
         <v>84.3</v>
       </c>
-      <c r="G10">
+      <c r="H10" s="1">
+        <f t="shared" si="1"/>
+        <v>109.21999999999998</v>
+      </c>
+      <c r="I10">
         <v>4.3</v>
       </c>
     </row>
-    <row r="11" spans="1:19">
+    <row r="11" spans="1:21">
       <c r="A11" t="s">
         <v>1</v>
       </c>
@@ -726,14 +811,22 @@
       <c r="E11">
         <v>201510</v>
       </c>
-      <c r="F11" s="1">
+      <c r="F11">
+        <f t="shared" si="0"/>
+        <v>29.222222222222221</v>
+      </c>
+      <c r="G11" s="1">
         <v>84.6</v>
       </c>
-      <c r="G11">
+      <c r="H11" s="1">
+        <f t="shared" si="1"/>
+        <v>44.957999999999998</v>
+      </c>
+      <c r="I11">
         <v>1.77</v>
       </c>
     </row>
-    <row r="12" spans="1:19">
+    <row r="12" spans="1:21">
       <c r="A12" t="s">
         <v>1</v>
       </c>
@@ -749,14 +842,22 @@
       <c r="E12">
         <v>201511</v>
       </c>
-      <c r="F12" s="1">
+      <c r="F12">
+        <f t="shared" si="0"/>
+        <v>27.333333333333332</v>
+      </c>
+      <c r="G12" s="1">
         <v>81.2</v>
       </c>
-      <c r="G12">
+      <c r="H12" s="1">
+        <f t="shared" si="1"/>
+        <v>221.488</v>
+      </c>
+      <c r="I12">
         <v>8.7200000000000006</v>
       </c>
     </row>
-    <row r="13" spans="1:19">
+    <row r="13" spans="1:21">
       <c r="A13" t="s">
         <v>1</v>
       </c>
@@ -772,14 +873,22 @@
       <c r="E13">
         <v>201512</v>
       </c>
-      <c r="F13" s="1">
+      <c r="F13">
+        <f t="shared" si="0"/>
+        <v>26.666666666666668</v>
+      </c>
+      <c r="G13" s="1">
         <v>80</v>
       </c>
-      <c r="G13">
+      <c r="H13" s="1">
+        <f t="shared" si="1"/>
+        <v>88.138000000000005</v>
+      </c>
+      <c r="I13">
         <v>3.47</v>
       </c>
     </row>
-    <row r="14" spans="1:19">
+    <row r="14" spans="1:21">
       <c r="A14" t="s">
         <v>7</v>
       </c>
@@ -796,13 +905,21 @@
         <v>201501</v>
       </c>
       <c r="F14">
+        <f t="shared" si="0"/>
+        <v>20.666666666666668</v>
+      </c>
+      <c r="G14">
         <v>69.2</v>
       </c>
-      <c r="G14" s="1">
+      <c r="H14" s="1">
+        <f t="shared" si="1"/>
+        <v>147.066</v>
+      </c>
+      <c r="I14" s="1">
         <v>5.79</v>
       </c>
     </row>
-    <row r="15" spans="1:19">
+    <row r="15" spans="1:21">
       <c r="A15" t="s">
         <v>7</v>
       </c>
@@ -819,13 +936,21 @@
         <v>201502</v>
       </c>
       <c r="F15">
+        <f t="shared" si="0"/>
+        <v>20.833333333333332</v>
+      </c>
+      <c r="G15">
         <v>69.5</v>
       </c>
-      <c r="G15" s="1">
+      <c r="H15" s="1">
+        <f t="shared" si="1"/>
+        <v>133.096</v>
+      </c>
+      <c r="I15" s="1">
         <v>5.24</v>
       </c>
     </row>
-    <row r="16" spans="1:19">
+    <row r="16" spans="1:21">
       <c r="A16" t="s">
         <v>7</v>
       </c>
@@ -842,13 +967,19 @@
         <v>201503</v>
       </c>
       <c r="F16">
+        <f t="shared" si="0"/>
+        <v>20.722222222222221</v>
+      </c>
+      <c r="G16">
         <v>69.3</v>
       </c>
-      <c r="G16" s="1">
+      <c r="H16" s="1">
+        <f t="shared" si="1"/>
+        <v>58.419999999999995</v>
+      </c>
+      <c r="I16" s="1">
         <v>2.2999999999999998</v>
       </c>
-      <c r="H16" s="1"/>
-      <c r="I16" s="1"/>
       <c r="J16" s="1"/>
       <c r="K16" s="1"/>
       <c r="L16" s="1"/>
@@ -859,8 +990,10 @@
       <c r="Q16" s="1"/>
       <c r="R16" s="1"/>
       <c r="S16" s="1"/>
-    </row>
-    <row r="17" spans="1:15">
+      <c r="T16" s="1"/>
+      <c r="U16" s="1"/>
+    </row>
+    <row r="17" spans="1:17">
       <c r="A17" t="s">
         <v>7</v>
       </c>
@@ -877,13 +1010,21 @@
         <v>201504</v>
       </c>
       <c r="F17">
+        <f t="shared" si="0"/>
+        <v>22.111111111111111</v>
+      </c>
+      <c r="G17">
         <v>71.8</v>
       </c>
-      <c r="G17" s="1">
+      <c r="H17" s="1">
+        <f t="shared" si="1"/>
+        <v>42.163999999999994</v>
+      </c>
+      <c r="I17" s="1">
         <v>1.66</v>
       </c>
     </row>
-    <row r="18" spans="1:15">
+    <row r="18" spans="1:17">
       <c r="A18" t="s">
         <v>7</v>
       </c>
@@ -900,13 +1041,21 @@
         <v>201505</v>
       </c>
       <c r="F18">
+        <f t="shared" si="0"/>
+        <v>23.166666666666668</v>
+      </c>
+      <c r="G18">
         <v>73.7</v>
       </c>
-      <c r="G18" s="1">
+      <c r="H18" s="1">
+        <f t="shared" si="1"/>
+        <v>113.28399999999999</v>
+      </c>
+      <c r="I18" s="1">
         <v>4.46</v>
       </c>
     </row>
-    <row r="19" spans="1:15">
+    <row r="19" spans="1:17">
       <c r="A19" t="s">
         <v>7</v>
       </c>
@@ -923,13 +1072,21 @@
         <v>201506</v>
       </c>
       <c r="F19">
+        <f t="shared" si="0"/>
+        <v>24.222222222222218</v>
+      </c>
+      <c r="G19">
         <v>75.599999999999994</v>
       </c>
-      <c r="G19" s="1">
+      <c r="H19" s="1">
+        <f t="shared" si="1"/>
+        <v>4.5719999999999992</v>
+      </c>
+      <c r="I19" s="1">
         <v>0.18</v>
       </c>
     </row>
-    <row r="20" spans="1:15">
+    <row r="20" spans="1:17">
       <c r="A20" t="s">
         <v>7</v>
       </c>
@@ -946,13 +1103,21 @@
         <v>201507</v>
       </c>
       <c r="F20">
+        <f t="shared" si="0"/>
+        <v>24.055555555555557</v>
+      </c>
+      <c r="G20">
         <v>75.3</v>
       </c>
-      <c r="G20" s="1">
+      <c r="H20" s="1">
+        <f t="shared" si="1"/>
+        <v>70.611999999999995</v>
+      </c>
+      <c r="I20" s="1">
         <v>2.78</v>
       </c>
     </row>
-    <row r="21" spans="1:15">
+    <row r="21" spans="1:17">
       <c r="A21" t="s">
         <v>7</v>
       </c>
@@ -969,13 +1134,21 @@
         <v>201508</v>
       </c>
       <c r="F21">
+        <f t="shared" si="0"/>
+        <v>24.499999999999996</v>
+      </c>
+      <c r="G21">
         <v>76.099999999999994</v>
       </c>
-      <c r="G21" s="1">
+      <c r="H21" s="1">
+        <f t="shared" si="1"/>
+        <v>124.46000000000001</v>
+      </c>
+      <c r="I21" s="1">
         <v>4.9000000000000004</v>
       </c>
     </row>
-    <row r="22" spans="1:15">
+    <row r="22" spans="1:17">
       <c r="A22" t="s">
         <v>7</v>
       </c>
@@ -992,13 +1165,21 @@
         <v>201509</v>
       </c>
       <c r="F22">
+        <f t="shared" si="0"/>
+        <v>24.222222222222218</v>
+      </c>
+      <c r="G22">
         <v>75.599999999999994</v>
       </c>
-      <c r="G22" s="1">
+      <c r="H22" s="1">
+        <f t="shared" si="1"/>
+        <v>174.244</v>
+      </c>
+      <c r="I22" s="1">
         <v>6.86</v>
       </c>
     </row>
-    <row r="23" spans="1:15">
+    <row r="23" spans="1:17">
       <c r="A23" t="s">
         <v>7</v>
       </c>
@@ -1015,13 +1196,21 @@
         <v>201510</v>
       </c>
       <c r="F23">
+        <f t="shared" si="0"/>
+        <v>23.5</v>
+      </c>
+      <c r="G23">
         <v>74.3</v>
       </c>
-      <c r="G23" s="1">
+      <c r="H23" s="1">
+        <f t="shared" si="1"/>
+        <v>353.56799999999998</v>
+      </c>
+      <c r="I23" s="1">
         <v>13.92</v>
       </c>
     </row>
-    <row r="24" spans="1:15">
+    <row r="24" spans="1:17">
       <c r="A24" t="s">
         <v>7</v>
       </c>
@@ -1038,13 +1227,21 @@
         <v>201511</v>
       </c>
       <c r="F24">
+        <f t="shared" si="0"/>
+        <v>22.111111111111111</v>
+      </c>
+      <c r="G24">
         <v>71.8</v>
       </c>
-      <c r="G24" s="1">
+      <c r="H24" s="1">
+        <f t="shared" si="1"/>
+        <v>173.73599999999999</v>
+      </c>
+      <c r="I24" s="1">
         <v>6.84</v>
       </c>
     </row>
-    <row r="25" spans="1:15">
+    <row r="25" spans="1:17">
       <c r="A25" t="s">
         <v>7</v>
       </c>
@@ -1061,13 +1258,21 @@
         <v>201512</v>
       </c>
       <c r="F25">
+        <f t="shared" si="0"/>
+        <v>21.388888888888889</v>
+      </c>
+      <c r="G25">
         <v>70.5</v>
       </c>
-      <c r="G25" s="1">
+      <c r="H25" s="1">
+        <f t="shared" si="1"/>
+        <v>86.105999999999995</v>
+      </c>
+      <c r="I25" s="1">
         <v>3.39</v>
       </c>
     </row>
-    <row r="26" spans="1:15">
+    <row r="26" spans="1:17">
       <c r="A26" t="s">
         <v>9</v>
       </c>
@@ -1084,13 +1289,21 @@
         <v>201501</v>
       </c>
       <c r="F26">
+        <f t="shared" si="0"/>
+        <v>21.611111111111114</v>
+      </c>
+      <c r="G26">
         <v>70.900000000000006</v>
       </c>
-      <c r="G26" s="1">
+      <c r="H26" s="1">
+        <f t="shared" si="1"/>
+        <v>35.051999999999992</v>
+      </c>
+      <c r="I26" s="1">
         <v>1.38</v>
       </c>
     </row>
-    <row r="27" spans="1:15">
+    <row r="27" spans="1:17">
       <c r="A27" t="s">
         <v>9</v>
       </c>
@@ -1109,11 +1322,18 @@
       <c r="F27">
         <v>-9999</v>
       </c>
-      <c r="G27" s="1">
+      <c r="G27">
+        <v>-9999</v>
+      </c>
+      <c r="H27" s="1">
+        <f t="shared" si="1"/>
+        <v>113.792</v>
+      </c>
+      <c r="I27" s="1">
         <v>4.4800000000000004</v>
       </c>
     </row>
-    <row r="28" spans="1:15">
+    <row r="28" spans="1:17">
       <c r="A28" t="s">
         <v>9</v>
       </c>
@@ -1132,19 +1352,26 @@
       <c r="F28">
         <v>-9999</v>
       </c>
-      <c r="G28" s="1">
+      <c r="G28">
+        <v>-9999</v>
+      </c>
+      <c r="H28" s="1">
+        <f t="shared" si="1"/>
+        <v>82.042000000000002</v>
+      </c>
+      <c r="I28" s="1">
         <v>3.23</v>
       </c>
-      <c r="H28" s="1"/>
-      <c r="I28" s="1"/>
       <c r="J28" s="1"/>
       <c r="K28" s="1"/>
       <c r="L28" s="1"/>
       <c r="M28" s="1"/>
       <c r="N28" s="1"/>
       <c r="O28" s="1"/>
-    </row>
-    <row r="29" spans="1:15">
+      <c r="P28" s="1"/>
+      <c r="Q28" s="1"/>
+    </row>
+    <row r="29" spans="1:17">
       <c r="A29" t="s">
         <v>9</v>
       </c>
@@ -1163,11 +1390,18 @@
       <c r="F29">
         <v>-9999</v>
       </c>
-      <c r="G29" s="1">
+      <c r="G29">
+        <v>-9999</v>
+      </c>
+      <c r="H29" s="1">
+        <f t="shared" si="1"/>
+        <v>248.15799999999999</v>
+      </c>
+      <c r="I29" s="1">
         <v>9.77</v>
       </c>
     </row>
-    <row r="30" spans="1:15">
+    <row r="30" spans="1:17">
       <c r="A30" t="s">
         <v>9</v>
       </c>
@@ -1184,13 +1418,21 @@
         <v>201505</v>
       </c>
       <c r="F30">
+        <f t="shared" si="0"/>
+        <v>24.388888888888893</v>
+      </c>
+      <c r="G30">
         <v>75.900000000000006</v>
       </c>
-      <c r="G30" s="1">
+      <c r="H30" s="1">
+        <f t="shared" si="1"/>
+        <v>227.07599999999996</v>
+      </c>
+      <c r="I30" s="1">
         <v>8.94</v>
       </c>
     </row>
-    <row r="31" spans="1:15">
+    <row r="31" spans="1:17">
       <c r="A31" t="s">
         <v>9</v>
       </c>
@@ -1207,13 +1449,21 @@
         <v>201506</v>
       </c>
       <c r="F31">
+        <f t="shared" si="0"/>
+        <v>25.500000000000004</v>
+      </c>
+      <c r="G31">
         <v>77.900000000000006</v>
       </c>
-      <c r="G31" s="1">
+      <c r="H31" s="1">
+        <f t="shared" si="1"/>
+        <v>253.49199999999999</v>
+      </c>
+      <c r="I31" s="1">
         <v>9.98</v>
       </c>
     </row>
-    <row r="32" spans="1:15">
+    <row r="32" spans="1:17">
       <c r="A32" t="s">
         <v>9</v>
       </c>
@@ -1232,11 +1482,18 @@
       <c r="F32">
         <v>-9999</v>
       </c>
-      <c r="G32" s="1">
+      <c r="G32">
+        <v>-9999</v>
+      </c>
+      <c r="H32" s="1">
+        <f t="shared" si="1"/>
+        <v>117.85599999999998</v>
+      </c>
+      <c r="I32" s="1">
         <v>4.6399999999999997</v>
       </c>
     </row>
-    <row r="33" spans="1:14">
+    <row r="33" spans="1:16">
       <c r="A33" t="s">
         <v>9</v>
       </c>
@@ -1255,11 +1512,18 @@
       <c r="F33">
         <v>-9999</v>
       </c>
-      <c r="G33" s="1">
+      <c r="G33">
+        <v>-9999</v>
+      </c>
+      <c r="H33" s="1">
+        <f t="shared" si="1"/>
+        <v>313.94399999999996</v>
+      </c>
+      <c r="I33" s="1">
         <v>12.36</v>
       </c>
     </row>
-    <row r="34" spans="1:14">
+    <row r="34" spans="1:16">
       <c r="A34" t="s">
         <v>9</v>
       </c>
@@ -1278,11 +1542,18 @@
       <c r="F34">
         <v>-9999</v>
       </c>
-      <c r="G34" s="1">
+      <c r="G34">
+        <v>-9999</v>
+      </c>
+      <c r="H34" s="1">
+        <f t="shared" si="1"/>
+        <v>361.95</v>
+      </c>
+      <c r="I34" s="1">
         <v>14.25</v>
       </c>
     </row>
-    <row r="35" spans="1:14">
+    <row r="35" spans="1:16">
       <c r="A35" t="s">
         <v>9</v>
       </c>
@@ -1299,13 +1570,21 @@
         <v>201510</v>
       </c>
       <c r="F35">
+        <f t="shared" si="0"/>
+        <v>25.333333333333329</v>
+      </c>
+      <c r="G35">
         <v>77.599999999999994</v>
       </c>
-      <c r="G35" s="1">
+      <c r="H35" s="1">
+        <f t="shared" si="1"/>
+        <v>161.036</v>
+      </c>
+      <c r="I35" s="1">
         <v>6.34</v>
       </c>
     </row>
-    <row r="36" spans="1:14">
+    <row r="36" spans="1:16">
       <c r="A36" t="s">
         <v>9</v>
       </c>
@@ -1324,11 +1603,18 @@
       <c r="F36">
         <v>-9999</v>
       </c>
-      <c r="G36" s="1">
+      <c r="G36">
+        <v>-9999</v>
+      </c>
+      <c r="H36" s="1">
+        <f t="shared" si="1"/>
+        <v>114.3</v>
+      </c>
+      <c r="I36" s="1">
         <v>4.5</v>
       </c>
     </row>
-    <row r="37" spans="1:14">
+    <row r="37" spans="1:16">
       <c r="A37" t="s">
         <v>9</v>
       </c>
@@ -1347,11 +1633,18 @@
       <c r="F37">
         <v>-9999</v>
       </c>
-      <c r="G37" s="1">
-        <v>-9999</v>
-      </c>
-    </row>
-    <row r="38" spans="1:14">
+      <c r="G37">
+        <v>-9999</v>
+      </c>
+      <c r="H37" s="1">
+        <f t="shared" si="1"/>
+        <v>-253974.59999999998</v>
+      </c>
+      <c r="I37" s="1">
+        <v>-9999</v>
+      </c>
+    </row>
+    <row r="38" spans="1:16">
       <c r="A38" t="s">
         <v>10</v>
       </c>
@@ -1367,14 +1660,22 @@
       <c r="E38">
         <v>201501</v>
       </c>
-      <c r="F38" s="1">
+      <c r="F38">
+        <f t="shared" si="0"/>
+        <v>24.444444444444443</v>
+      </c>
+      <c r="G38" s="1">
         <v>76</v>
       </c>
-      <c r="G38" s="1">
+      <c r="H38" s="1">
+        <f t="shared" si="1"/>
+        <v>95.25</v>
+      </c>
+      <c r="I38" s="1">
         <v>3.75</v>
       </c>
     </row>
-    <row r="39" spans="1:14">
+    <row r="39" spans="1:16">
       <c r="A39" t="s">
         <v>10</v>
       </c>
@@ -1390,21 +1691,29 @@
       <c r="E39">
         <v>201502</v>
       </c>
-      <c r="F39" s="1">
+      <c r="F39">
+        <f t="shared" si="0"/>
+        <v>25</v>
+      </c>
+      <c r="G39" s="1">
         <v>77</v>
       </c>
-      <c r="G39" s="1">
+      <c r="H39" s="1">
+        <f t="shared" si="1"/>
+        <v>168.40199999999999</v>
+      </c>
+      <c r="I39" s="1">
         <v>6.63</v>
       </c>
-      <c r="H39" s="1"/>
-      <c r="I39" s="1"/>
       <c r="J39" s="1"/>
       <c r="K39" s="1"/>
       <c r="L39" s="1"/>
       <c r="M39" s="1"/>
       <c r="N39" s="1"/>
-    </row>
-    <row r="40" spans="1:14">
+      <c r="O39" s="1"/>
+      <c r="P39" s="1"/>
+    </row>
+    <row r="40" spans="1:16">
       <c r="A40" t="s">
         <v>10</v>
       </c>
@@ -1420,14 +1729,22 @@
       <c r="E40">
         <v>201503</v>
       </c>
-      <c r="F40" s="1">
+      <c r="F40">
+        <f t="shared" si="0"/>
+        <v>24.722222222222221</v>
+      </c>
+      <c r="G40" s="1">
         <v>76.5</v>
       </c>
-      <c r="G40" s="1">
+      <c r="H40" s="1">
+        <f t="shared" si="1"/>
+        <v>39.369999999999997</v>
+      </c>
+      <c r="I40" s="1">
         <v>1.55</v>
       </c>
     </row>
-    <row r="41" spans="1:14">
+    <row r="41" spans="1:16">
       <c r="A41" t="s">
         <v>10</v>
       </c>
@@ -1443,14 +1760,22 @@
       <c r="E41">
         <v>201504</v>
       </c>
-      <c r="F41" s="1">
+      <c r="F41">
+        <f t="shared" si="0"/>
+        <v>25.611111111111107</v>
+      </c>
+      <c r="G41" s="1">
         <v>78.099999999999994</v>
       </c>
-      <c r="G41" s="1">
+      <c r="H41" s="1">
+        <f t="shared" si="1"/>
+        <v>187.19799999999998</v>
+      </c>
+      <c r="I41" s="1">
         <v>7.37</v>
       </c>
     </row>
-    <row r="42" spans="1:14">
+    <row r="42" spans="1:16">
       <c r="A42" t="s">
         <v>10</v>
       </c>
@@ -1466,14 +1791,22 @@
       <c r="E42">
         <v>201505</v>
       </c>
-      <c r="F42" s="1">
+      <c r="F42">
+        <f t="shared" si="0"/>
+        <v>26.555555555555557</v>
+      </c>
+      <c r="G42" s="1">
         <v>79.8</v>
       </c>
-      <c r="G42" s="1">
+      <c r="H42" s="1">
+        <f t="shared" si="1"/>
+        <v>184.14999999999998</v>
+      </c>
+      <c r="I42" s="1">
         <v>7.25</v>
       </c>
     </row>
-    <row r="43" spans="1:14">
+    <row r="43" spans="1:16">
       <c r="A43" t="s">
         <v>10</v>
       </c>
@@ -1489,14 +1822,22 @@
       <c r="E43">
         <v>201506</v>
       </c>
-      <c r="F43" s="1">
+      <c r="F43">
+        <f t="shared" si="0"/>
+        <v>27.111111111111111</v>
+      </c>
+      <c r="G43" s="1">
         <v>80.8</v>
       </c>
-      <c r="G43" s="1">
+      <c r="H43" s="1">
+        <f t="shared" si="1"/>
+        <v>124.96799999999999</v>
+      </c>
+      <c r="I43" s="1">
         <v>4.92</v>
       </c>
     </row>
-    <row r="44" spans="1:14">
+    <row r="44" spans="1:16">
       <c r="A44" t="s">
         <v>10</v>
       </c>
@@ -1512,14 +1853,22 @@
       <c r="E44">
         <v>201507</v>
       </c>
-      <c r="F44" s="1">
+      <c r="F44">
+        <f t="shared" si="0"/>
+        <v>27.166666666666671</v>
+      </c>
+      <c r="G44" s="1">
         <v>80.900000000000006</v>
       </c>
-      <c r="G44" s="1">
+      <c r="H44" s="1">
+        <f t="shared" si="1"/>
+        <v>108.96599999999999</v>
+      </c>
+      <c r="I44" s="1">
         <v>4.29</v>
       </c>
     </row>
-    <row r="45" spans="1:14">
+    <row r="45" spans="1:16">
       <c r="A45" t="s">
         <v>10</v>
       </c>
@@ -1535,14 +1884,22 @@
       <c r="E45">
         <v>201508</v>
       </c>
-      <c r="F45" s="1">
+      <c r="F45">
+        <f t="shared" si="0"/>
+        <v>27.333333333333332</v>
+      </c>
+      <c r="G45" s="1">
         <v>81.2</v>
       </c>
-      <c r="G45" s="1">
+      <c r="H45" s="1">
+        <f t="shared" si="1"/>
+        <v>212.852</v>
+      </c>
+      <c r="I45" s="1">
         <v>8.3800000000000008</v>
       </c>
     </row>
-    <row r="46" spans="1:14">
+    <row r="46" spans="1:16">
       <c r="A46" t="s">
         <v>10</v>
       </c>
@@ -1558,14 +1915,22 @@
       <c r="E46">
         <v>201509</v>
       </c>
-      <c r="F46" s="1">
+      <c r="F46">
+        <f t="shared" si="0"/>
+        <v>27.666666666666668</v>
+      </c>
+      <c r="G46" s="1">
         <v>81.8</v>
       </c>
-      <c r="G46" s="1">
+      <c r="H46" s="1">
+        <f t="shared" si="1"/>
+        <v>274.06599999999997</v>
+      </c>
+      <c r="I46" s="1">
         <v>10.79</v>
       </c>
     </row>
-    <row r="47" spans="1:14">
+    <row r="47" spans="1:16">
       <c r="A47" t="s">
         <v>10</v>
       </c>
@@ -1581,14 +1946,22 @@
       <c r="E47">
         <v>201510</v>
       </c>
-      <c r="F47" s="1">
+      <c r="F47">
+        <f t="shared" si="0"/>
+        <v>27.666666666666668</v>
+      </c>
+      <c r="G47" s="1">
         <v>81.8</v>
       </c>
-      <c r="G47" s="1">
+      <c r="H47" s="1">
+        <f t="shared" si="1"/>
+        <v>197.10399999999998</v>
+      </c>
+      <c r="I47" s="1">
         <v>7.76</v>
       </c>
     </row>
-    <row r="48" spans="1:14">
+    <row r="48" spans="1:16">
       <c r="A48" t="s">
         <v>10</v>
       </c>
@@ -1604,14 +1977,22 @@
       <c r="E48">
         <v>201511</v>
       </c>
-      <c r="F48" s="1">
+      <c r="F48">
+        <f t="shared" si="0"/>
+        <v>25.833333333333332</v>
+      </c>
+      <c r="G48" s="1">
         <v>78.5</v>
       </c>
-      <c r="G48" s="1">
+      <c r="H48" s="1">
+        <f t="shared" si="1"/>
+        <v>135.12799999999999</v>
+      </c>
+      <c r="I48" s="1">
         <v>5.32</v>
       </c>
     </row>
-    <row r="49" spans="1:13">
+    <row r="49" spans="1:15">
       <c r="A49" t="s">
         <v>10</v>
       </c>
@@ -1627,14 +2008,22 @@
       <c r="E49">
         <v>201512</v>
       </c>
-      <c r="F49" s="1">
+      <c r="F49">
+        <f t="shared" si="0"/>
+        <v>25.222222222222225</v>
+      </c>
+      <c r="G49" s="1">
         <v>77.400000000000006</v>
       </c>
-      <c r="G49" s="1">
-        <v>-9999</v>
-      </c>
-    </row>
-    <row r="50" spans="1:13">
+      <c r="H49" s="1">
+        <f t="shared" si="1"/>
+        <v>-253974.59999999998</v>
+      </c>
+      <c r="I49" s="1">
+        <v>-9999</v>
+      </c>
+    </row>
+    <row r="50" spans="1:15">
       <c r="A50" t="s">
         <v>11</v>
       </c>
@@ -1653,11 +2042,18 @@
       <c r="F50" s="1">
         <v>-9999</v>
       </c>
-      <c r="G50">
+      <c r="G50" s="1">
+        <v>-9999</v>
+      </c>
+      <c r="H50" s="1">
+        <f t="shared" si="1"/>
+        <v>53.339999999999996</v>
+      </c>
+      <c r="I50">
         <v>2.1</v>
       </c>
     </row>
-    <row r="51" spans="1:13">
+    <row r="51" spans="1:15">
       <c r="A51" t="s">
         <v>11</v>
       </c>
@@ -1676,17 +2072,24 @@
       <c r="F51" s="1">
         <v>-9999</v>
       </c>
-      <c r="G51">
+      <c r="G51" s="1">
+        <v>-9999</v>
+      </c>
+      <c r="H51" s="1">
+        <f t="shared" si="1"/>
+        <v>41.401999999999994</v>
+      </c>
+      <c r="I51">
         <v>1.63</v>
       </c>
-      <c r="H51" s="1"/>
-      <c r="I51" s="1"/>
       <c r="J51" s="1"/>
       <c r="K51" s="1"/>
       <c r="L51" s="1"/>
       <c r="M51" s="1"/>
-    </row>
-    <row r="52" spans="1:13">
+      <c r="N51" s="1"/>
+      <c r="O51" s="1"/>
+    </row>
+    <row r="52" spans="1:15">
       <c r="A52" t="s">
         <v>11</v>
       </c>
@@ -1705,11 +2108,18 @@
       <c r="F52" s="1">
         <v>-9999</v>
       </c>
-      <c r="G52">
+      <c r="G52" s="1">
+        <v>-9999</v>
+      </c>
+      <c r="H52" s="1">
+        <f t="shared" si="1"/>
+        <v>44.957999999999998</v>
+      </c>
+      <c r="I52">
         <v>1.77</v>
       </c>
     </row>
-    <row r="53" spans="1:13">
+    <row r="53" spans="1:15">
       <c r="A53" t="s">
         <v>11</v>
       </c>
@@ -1728,11 +2138,18 @@
       <c r="F53" s="1">
         <v>-9999</v>
       </c>
-      <c r="G53">
+      <c r="G53" s="1">
+        <v>-9999</v>
+      </c>
+      <c r="H53" s="1">
+        <f t="shared" si="1"/>
+        <v>22.352</v>
+      </c>
+      <c r="I53">
         <v>0.88</v>
       </c>
     </row>
-    <row r="54" spans="1:13">
+    <row r="54" spans="1:15">
       <c r="A54" t="s">
         <v>11</v>
       </c>
@@ -1751,11 +2168,18 @@
       <c r="F54" s="1">
         <v>-9999</v>
       </c>
-      <c r="G54">
+      <c r="G54" s="1">
+        <v>-9999</v>
+      </c>
+      <c r="H54" s="1">
+        <f t="shared" si="1"/>
+        <v>48.767999999999994</v>
+      </c>
+      <c r="I54">
         <v>1.92</v>
       </c>
     </row>
-    <row r="55" spans="1:13">
+    <row r="55" spans="1:15">
       <c r="A55" t="s">
         <v>11</v>
       </c>
@@ -1774,11 +2198,18 @@
       <c r="F55" s="1">
         <v>-9999</v>
       </c>
-      <c r="G55">
+      <c r="G55" s="1">
+        <v>-9999</v>
+      </c>
+      <c r="H55" s="1">
+        <f t="shared" si="1"/>
+        <v>3.0479999999999996</v>
+      </c>
+      <c r="I55">
         <v>0.12</v>
       </c>
     </row>
-    <row r="56" spans="1:13">
+    <row r="56" spans="1:15">
       <c r="A56" t="s">
         <v>11</v>
       </c>
@@ -1797,11 +2228,18 @@
       <c r="F56" s="1">
         <v>-9999</v>
       </c>
-      <c r="G56">
+      <c r="G56" s="1">
+        <v>-9999</v>
+      </c>
+      <c r="H56" s="1">
+        <f t="shared" si="1"/>
+        <v>37.591999999999999</v>
+      </c>
+      <c r="I56">
         <v>1.48</v>
       </c>
     </row>
-    <row r="57" spans="1:13">
+    <row r="57" spans="1:15">
       <c r="A57" t="s">
         <v>11</v>
       </c>
@@ -1820,11 +2258,18 @@
       <c r="F57" s="1">
         <v>-9999</v>
       </c>
-      <c r="G57">
+      <c r="G57" s="1">
+        <v>-9999</v>
+      </c>
+      <c r="H57" s="1">
+        <f t="shared" si="1"/>
+        <v>92.963999999999999</v>
+      </c>
+      <c r="I57">
         <v>3.66</v>
       </c>
     </row>
-    <row r="58" spans="1:13">
+    <row r="58" spans="1:15">
       <c r="A58" t="s">
         <v>11</v>
       </c>
@@ -1843,11 +2288,18 @@
       <c r="F58" s="1">
         <v>-9999</v>
       </c>
-      <c r="G58">
+      <c r="G58" s="1">
+        <v>-9999</v>
+      </c>
+      <c r="H58" s="1">
+        <f t="shared" si="1"/>
+        <v>38.099999999999994</v>
+      </c>
+      <c r="I58">
         <v>1.5</v>
       </c>
     </row>
-    <row r="59" spans="1:13">
+    <row r="59" spans="1:15">
       <c r="A59" t="s">
         <v>11</v>
       </c>
@@ -1866,11 +2318,18 @@
       <c r="F59" s="1">
         <v>-9999</v>
       </c>
-      <c r="G59">
+      <c r="G59" s="1">
+        <v>-9999</v>
+      </c>
+      <c r="H59" s="1">
+        <f t="shared" si="1"/>
+        <v>44.704000000000001</v>
+      </c>
+      <c r="I59">
         <v>1.76</v>
       </c>
     </row>
-    <row r="60" spans="1:13">
+    <row r="60" spans="1:15">
       <c r="A60" t="s">
         <v>11</v>
       </c>
@@ -1889,11 +2348,18 @@
       <c r="F60" s="1">
         <v>-9999</v>
       </c>
-      <c r="G60">
+      <c r="G60" s="1">
+        <v>-9999</v>
+      </c>
+      <c r="H60" s="1">
+        <f t="shared" si="1"/>
+        <v>88.899999999999991</v>
+      </c>
+      <c r="I60">
         <v>3.5</v>
       </c>
     </row>
-    <row r="61" spans="1:13">
+    <row r="61" spans="1:15">
       <c r="A61" t="s">
         <v>11</v>
       </c>
@@ -1912,11 +2378,18 @@
       <c r="F61" s="1">
         <v>-9999</v>
       </c>
-      <c r="G61">
+      <c r="G61" s="1">
+        <v>-9999</v>
+      </c>
+      <c r="H61" s="1">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="62" spans="1:13">
+      <c r="I61">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62" spans="1:15">
       <c r="A62" t="s">
         <v>12</v>
       </c>
@@ -1932,14 +2405,22 @@
       <c r="E62">
         <v>201501</v>
       </c>
-      <c r="F62" s="1">
+      <c r="F62">
+        <f t="shared" si="0"/>
+        <v>26.722222222222218</v>
+      </c>
+      <c r="G62" s="1">
         <v>80.099999999999994</v>
       </c>
-      <c r="G62" s="1">
+      <c r="H62" s="1">
+        <f t="shared" si="1"/>
+        <v>43.942</v>
+      </c>
+      <c r="I62" s="1">
         <v>1.73</v>
       </c>
     </row>
-    <row r="63" spans="1:13">
+    <row r="63" spans="1:15">
       <c r="A63" t="s">
         <v>12</v>
       </c>
@@ -1955,14 +2436,22 @@
       <c r="E63">
         <v>201502</v>
       </c>
-      <c r="F63" s="1">
+      <c r="F63">
+        <f t="shared" si="0"/>
+        <v>27.055555555555557</v>
+      </c>
+      <c r="G63" s="1">
         <v>80.7</v>
       </c>
-      <c r="G63" s="1">
+      <c r="H63" s="1">
+        <f t="shared" si="1"/>
+        <v>56.896000000000001</v>
+      </c>
+      <c r="I63" s="1">
         <v>2.2400000000000002</v>
       </c>
     </row>
-    <row r="64" spans="1:13">
+    <row r="64" spans="1:15">
       <c r="A64" t="s">
         <v>12</v>
       </c>
@@ -1978,14 +2467,22 @@
       <c r="E64">
         <v>201503</v>
       </c>
-      <c r="F64" s="1">
+      <c r="F64">
+        <f t="shared" si="0"/>
+        <v>26.722222222222218</v>
+      </c>
+      <c r="G64" s="1">
         <v>80.099999999999994</v>
       </c>
-      <c r="G64" s="1">
+      <c r="H64" s="1">
+        <f t="shared" si="1"/>
+        <v>31.75</v>
+      </c>
+      <c r="I64" s="1">
         <v>1.25</v>
       </c>
     </row>
-    <row r="65" spans="1:18">
+    <row r="65" spans="1:20">
       <c r="A65" t="s">
         <v>12</v>
       </c>
@@ -2001,14 +2498,22 @@
       <c r="E65">
         <v>201504</v>
       </c>
-      <c r="F65" s="1">
+      <c r="F65">
+        <f t="shared" si="0"/>
+        <v>27.611111111111111</v>
+      </c>
+      <c r="G65" s="1">
         <v>81.7</v>
       </c>
-      <c r="G65" s="1">
+      <c r="H65" s="1">
+        <f t="shared" si="1"/>
+        <v>22.86</v>
+      </c>
+      <c r="I65" s="1">
         <v>0.9</v>
       </c>
     </row>
-    <row r="66" spans="1:18">
+    <row r="66" spans="1:20">
       <c r="A66" t="s">
         <v>12</v>
       </c>
@@ -2024,14 +2529,22 @@
       <c r="E66">
         <v>201505</v>
       </c>
-      <c r="F66" s="1">
+      <c r="F66">
+        <f t="shared" si="0"/>
+        <v>28.777777777777779</v>
+      </c>
+      <c r="G66" s="1">
         <v>83.8</v>
       </c>
-      <c r="G66" s="1">
+      <c r="H66" s="1">
+        <f t="shared" si="1"/>
+        <v>6.8579999999999997</v>
+      </c>
+      <c r="I66" s="1">
         <v>0.27</v>
       </c>
     </row>
-    <row r="67" spans="1:18">
+    <row r="67" spans="1:20">
       <c r="A67" t="s">
         <v>12</v>
       </c>
@@ -2047,14 +2560,22 @@
       <c r="E67">
         <v>201506</v>
       </c>
-      <c r="F67" s="1">
+      <c r="F67">
+        <f t="shared" ref="F67:F130" si="2">(G67-32)*5/9</f>
+        <v>29.666666666666668</v>
+      </c>
+      <c r="G67" s="1">
         <v>85.4</v>
       </c>
-      <c r="G67" s="1">
+      <c r="H67" s="1">
+        <f t="shared" ref="H67:H130" si="3">I67*25.4</f>
+        <v>23.367999999999999</v>
+      </c>
+      <c r="I67" s="1">
         <v>0.92</v>
       </c>
     </row>
-    <row r="68" spans="1:18">
+    <row r="68" spans="1:20">
       <c r="A68" t="s">
         <v>12</v>
       </c>
@@ -2070,14 +2591,22 @@
       <c r="E68">
         <v>201507</v>
       </c>
-      <c r="F68" s="1">
+      <c r="F68">
+        <f t="shared" si="2"/>
+        <v>28.888888888888889</v>
+      </c>
+      <c r="G68" s="1">
         <v>84</v>
       </c>
-      <c r="G68" s="1">
+      <c r="H68" s="1">
+        <f t="shared" si="3"/>
+        <v>75.691999999999993</v>
+      </c>
+      <c r="I68" s="1">
         <v>2.98</v>
       </c>
     </row>
-    <row r="69" spans="1:18">
+    <row r="69" spans="1:20">
       <c r="A69" t="s">
         <v>12</v>
       </c>
@@ -2093,14 +2622,22 @@
       <c r="E69">
         <v>201508</v>
       </c>
-      <c r="F69" s="1">
+      <c r="F69">
+        <f t="shared" si="2"/>
+        <v>29.166666666666668</v>
+      </c>
+      <c r="G69" s="1">
         <v>84.5</v>
       </c>
-      <c r="G69" s="1">
+      <c r="H69" s="1">
+        <f t="shared" si="3"/>
+        <v>106.17199999999998</v>
+      </c>
+      <c r="I69" s="1">
         <v>4.18</v>
       </c>
     </row>
-    <row r="70" spans="1:18">
+    <row r="70" spans="1:20">
       <c r="A70" t="s">
         <v>12</v>
       </c>
@@ -2116,14 +2653,22 @@
       <c r="E70">
         <v>201509</v>
       </c>
-      <c r="F70" s="1">
+      <c r="F70">
+        <f t="shared" si="2"/>
+        <v>29.277777777777779</v>
+      </c>
+      <c r="G70" s="1">
         <v>84.7</v>
       </c>
-      <c r="G70" s="1">
+      <c r="H70" s="1">
+        <f t="shared" si="3"/>
+        <v>45.973999999999997</v>
+      </c>
+      <c r="I70" s="1">
         <v>1.81</v>
       </c>
     </row>
-    <row r="71" spans="1:18">
+    <row r="71" spans="1:20">
       <c r="A71" t="s">
         <v>12</v>
       </c>
@@ -2139,14 +2684,22 @@
       <c r="E71">
         <v>201510</v>
       </c>
-      <c r="F71" s="1">
+      <c r="F71">
+        <f t="shared" si="2"/>
+        <v>29.277777777777779</v>
+      </c>
+      <c r="G71" s="1">
         <v>84.7</v>
       </c>
-      <c r="G71" s="1">
+      <c r="H71" s="1">
+        <f t="shared" si="3"/>
+        <v>122.93599999999999</v>
+      </c>
+      <c r="I71" s="1">
         <v>4.84</v>
       </c>
     </row>
-    <row r="72" spans="1:18">
+    <row r="72" spans="1:20">
       <c r="A72" t="s">
         <v>12</v>
       </c>
@@ -2162,14 +2715,22 @@
       <c r="E72">
         <v>201511</v>
       </c>
-      <c r="F72" s="1">
+      <c r="F72">
+        <f t="shared" si="2"/>
+        <v>27.166666666666671</v>
+      </c>
+      <c r="G72" s="1">
         <v>80.900000000000006</v>
       </c>
-      <c r="G72" s="1">
+      <c r="H72" s="1">
+        <f t="shared" si="3"/>
+        <v>249.93599999999998</v>
+      </c>
+      <c r="I72" s="1">
         <v>9.84</v>
       </c>
     </row>
-    <row r="73" spans="1:18">
+    <row r="73" spans="1:20">
       <c r="A73" t="s">
         <v>12</v>
       </c>
@@ -2185,14 +2746,22 @@
       <c r="E73">
         <v>201512</v>
       </c>
-      <c r="F73" s="1">
+      <c r="F73">
+        <f t="shared" si="2"/>
+        <v>27.833333333333329</v>
+      </c>
+      <c r="G73" s="1">
         <v>82.1</v>
       </c>
-      <c r="G73" s="1">
+      <c r="H73" s="1">
+        <f t="shared" si="3"/>
+        <v>78.48599999999999</v>
+      </c>
+      <c r="I73" s="1">
         <v>3.09</v>
       </c>
     </row>
-    <row r="74" spans="1:18">
+    <row r="74" spans="1:20">
       <c r="A74" t="s">
         <v>13</v>
       </c>
@@ -2208,14 +2777,22 @@
       <c r="E74">
         <v>201501</v>
       </c>
-      <c r="F74" s="1">
+      <c r="F74">
+        <f t="shared" si="2"/>
+        <v>25.111111111111111</v>
+      </c>
+      <c r="G74" s="1">
         <v>77.2</v>
       </c>
-      <c r="G74" s="1">
+      <c r="H74" s="1">
+        <f t="shared" si="3"/>
+        <v>61.467999999999996</v>
+      </c>
+      <c r="I74" s="1">
         <v>2.42</v>
       </c>
     </row>
-    <row r="75" spans="1:18">
+    <row r="75" spans="1:20">
       <c r="A75" t="s">
         <v>13</v>
       </c>
@@ -2231,14 +2808,20 @@
       <c r="E75">
         <v>201502</v>
       </c>
-      <c r="F75" s="1">
+      <c r="F75">
+        <f t="shared" si="2"/>
+        <v>25.333333333333329</v>
+      </c>
+      <c r="G75" s="1">
         <v>77.599999999999994</v>
       </c>
-      <c r="G75" s="1">
+      <c r="H75" s="1">
+        <f t="shared" si="3"/>
+        <v>100.58399999999999</v>
+      </c>
+      <c r="I75" s="1">
         <v>3.96</v>
       </c>
-      <c r="H75" s="1"/>
-      <c r="I75" s="1"/>
       <c r="J75" s="1"/>
       <c r="K75" s="1"/>
       <c r="L75" s="1"/>
@@ -2248,8 +2831,10 @@
       <c r="P75" s="1"/>
       <c r="Q75" s="1"/>
       <c r="R75" s="1"/>
-    </row>
-    <row r="76" spans="1:18">
+      <c r="S75" s="1"/>
+      <c r="T75" s="1"/>
+    </row>
+    <row r="76" spans="1:20">
       <c r="A76" t="s">
         <v>13</v>
       </c>
@@ -2265,14 +2850,22 @@
       <c r="E76">
         <v>201503</v>
       </c>
-      <c r="F76" s="1">
+      <c r="F76">
+        <f t="shared" si="2"/>
+        <v>25.166666666666668</v>
+      </c>
+      <c r="G76" s="1">
         <v>77.3</v>
       </c>
-      <c r="G76" s="1">
+      <c r="H76" s="1">
+        <f t="shared" si="3"/>
+        <v>47.751999999999995</v>
+      </c>
+      <c r="I76" s="1">
         <v>1.88</v>
       </c>
     </row>
-    <row r="77" spans="1:18">
+    <row r="77" spans="1:20">
       <c r="A77" t="s">
         <v>13</v>
       </c>
@@ -2288,14 +2881,22 @@
       <c r="E77">
         <v>201504</v>
       </c>
-      <c r="F77" s="1">
+      <c r="F77">
+        <f t="shared" si="2"/>
+        <v>26.444444444444443</v>
+      </c>
+      <c r="G77" s="1">
         <v>79.599999999999994</v>
       </c>
-      <c r="G77" s="1">
+      <c r="H77" s="1">
+        <f t="shared" si="3"/>
+        <v>60.959999999999994</v>
+      </c>
+      <c r="I77" s="1">
         <v>2.4</v>
       </c>
     </row>
-    <row r="78" spans="1:18">
+    <row r="78" spans="1:20">
       <c r="A78" t="s">
         <v>13</v>
       </c>
@@ -2311,14 +2912,22 @@
       <c r="E78">
         <v>201505</v>
       </c>
-      <c r="F78" s="1">
+      <c r="F78">
+        <f t="shared" si="2"/>
+        <v>27.666666666666668</v>
+      </c>
+      <c r="G78" s="1">
         <v>81.8</v>
       </c>
-      <c r="G78" s="1">
+      <c r="H78" s="1">
+        <f t="shared" si="3"/>
+        <v>88.899999999999991</v>
+      </c>
+      <c r="I78" s="1">
         <v>3.5</v>
       </c>
     </row>
-    <row r="79" spans="1:18">
+    <row r="79" spans="1:20">
       <c r="A79" t="s">
         <v>13</v>
       </c>
@@ -2334,19 +2943,27 @@
       <c r="E79">
         <v>201506</v>
       </c>
-      <c r="F79" s="1">
+      <c r="F79">
+        <f t="shared" si="2"/>
+        <v>28.055555555555557</v>
+      </c>
+      <c r="G79" s="1">
         <v>82.5</v>
       </c>
-      <c r="G79" s="1">
+      <c r="H79" s="1">
+        <f t="shared" si="3"/>
+        <v>52.832000000000001</v>
+      </c>
+      <c r="I79" s="1">
         <v>2.08</v>
       </c>
-      <c r="H79" s="1"/>
-      <c r="I79" s="1"/>
       <c r="J79" s="1"/>
       <c r="K79" s="1"/>
       <c r="L79" s="1"/>
-    </row>
-    <row r="80" spans="1:18">
+      <c r="M79" s="1"/>
+      <c r="N79" s="1"/>
+    </row>
+    <row r="80" spans="1:20">
       <c r="A80" t="s">
         <v>13</v>
       </c>
@@ -2362,14 +2979,22 @@
       <c r="E80">
         <v>201507</v>
       </c>
-      <c r="F80" s="1">
+      <c r="F80">
+        <f t="shared" si="2"/>
+        <v>28.000000000000004</v>
+      </c>
+      <c r="G80" s="1">
         <v>82.4</v>
       </c>
-      <c r="G80" s="1">
+      <c r="H80" s="1">
+        <f t="shared" si="3"/>
+        <v>40.64</v>
+      </c>
+      <c r="I80" s="1">
         <v>1.6</v>
       </c>
     </row>
-    <row r="81" spans="1:14">
+    <row r="81" spans="1:16">
       <c r="A81" t="s">
         <v>13</v>
       </c>
@@ -2385,14 +3010,22 @@
       <c r="E81">
         <v>201508</v>
       </c>
-      <c r="F81" s="1">
+      <c r="F81">
+        <f t="shared" si="2"/>
+        <v>28.166666666666668</v>
+      </c>
+      <c r="G81" s="1">
         <v>82.7</v>
       </c>
-      <c r="G81" s="1">
+      <c r="H81" s="1">
+        <f t="shared" si="3"/>
+        <v>101.85399999999998</v>
+      </c>
+      <c r="I81" s="1">
         <v>4.01</v>
       </c>
     </row>
-    <row r="82" spans="1:14">
+    <row r="82" spans="1:16">
       <c r="A82" t="s">
         <v>13</v>
       </c>
@@ -2408,14 +3041,22 @@
       <c r="E82">
         <v>201509</v>
       </c>
-      <c r="F82" s="1">
+      <c r="F82">
+        <f t="shared" si="2"/>
+        <v>27.833333333333329</v>
+      </c>
+      <c r="G82" s="1">
         <v>82.1</v>
       </c>
-      <c r="G82" s="1">
+      <c r="H82" s="1">
+        <f t="shared" si="3"/>
+        <v>154.43199999999999</v>
+      </c>
+      <c r="I82" s="1">
         <v>6.08</v>
       </c>
     </row>
-    <row r="83" spans="1:14">
+    <row r="83" spans="1:16">
       <c r="A83" t="s">
         <v>13</v>
       </c>
@@ -2431,14 +3072,22 @@
       <c r="E83">
         <v>201510</v>
       </c>
-      <c r="F83" s="1">
+      <c r="F83">
+        <f t="shared" si="2"/>
+        <v>27.777777777777779</v>
+      </c>
+      <c r="G83" s="1">
         <v>82</v>
       </c>
-      <c r="G83" s="1">
+      <c r="H83" s="1">
+        <f t="shared" si="3"/>
+        <v>148.58999999999997</v>
+      </c>
+      <c r="I83" s="1">
         <v>5.85</v>
       </c>
     </row>
-    <row r="84" spans="1:14">
+    <row r="84" spans="1:16">
       <c r="A84" t="s">
         <v>13</v>
       </c>
@@ -2454,14 +3103,22 @@
       <c r="E84">
         <v>201511</v>
       </c>
-      <c r="F84" s="1">
+      <c r="F84">
+        <f t="shared" si="2"/>
+        <v>26.277777777777779</v>
+      </c>
+      <c r="G84" s="1">
         <v>79.3</v>
       </c>
-      <c r="G84" s="1">
+      <c r="H84" s="1">
+        <f t="shared" si="3"/>
+        <v>292.60799999999995</v>
+      </c>
+      <c r="I84" s="1">
         <v>11.52</v>
       </c>
     </row>
-    <row r="85" spans="1:14">
+    <row r="85" spans="1:16">
       <c r="A85" t="s">
         <v>13</v>
       </c>
@@ -2477,14 +3134,22 @@
       <c r="E85">
         <v>201512</v>
       </c>
-      <c r="F85" s="1">
+      <c r="F85">
+        <f t="shared" si="2"/>
+        <v>26.055555555555557</v>
+      </c>
+      <c r="G85" s="1">
         <v>78.900000000000006</v>
       </c>
-      <c r="G85" s="1">
+      <c r="H85" s="1">
+        <f t="shared" si="3"/>
+        <v>182.626</v>
+      </c>
+      <c r="I85" s="1">
         <v>7.19</v>
       </c>
     </row>
-    <row r="86" spans="1:14">
+    <row r="86" spans="1:16">
       <c r="A86" t="s">
         <v>14</v>
       </c>
@@ -2500,14 +3165,22 @@
       <c r="E86">
         <v>201501</v>
       </c>
-      <c r="F86" s="1">
+      <c r="F86">
+        <f t="shared" si="2"/>
+        <v>24.499999999999996</v>
+      </c>
+      <c r="G86" s="1">
         <v>76.099999999999994</v>
       </c>
-      <c r="G86" s="1">
+      <c r="H86" s="1">
+        <f t="shared" si="3"/>
+        <v>83.82</v>
+      </c>
+      <c r="I86" s="1">
         <v>3.3</v>
       </c>
     </row>
-    <row r="87" spans="1:14">
+    <row r="87" spans="1:16">
       <c r="A87" t="s">
         <v>14</v>
       </c>
@@ -2523,21 +3196,29 @@
       <c r="E87">
         <v>201502</v>
       </c>
-      <c r="F87" s="1">
+      <c r="F87">
+        <f t="shared" si="2"/>
+        <v>24.888888888888889</v>
+      </c>
+      <c r="G87" s="1">
         <v>76.8</v>
       </c>
-      <c r="G87" s="1">
+      <c r="H87" s="1">
+        <f t="shared" si="3"/>
+        <v>81.025999999999996</v>
+      </c>
+      <c r="I87" s="1">
         <v>3.19</v>
       </c>
-      <c r="H87" s="1"/>
-      <c r="I87" s="1"/>
       <c r="J87" s="1"/>
       <c r="K87" s="1"/>
       <c r="L87" s="1"/>
       <c r="M87" s="1"/>
       <c r="N87" s="1"/>
-    </row>
-    <row r="88" spans="1:14">
+      <c r="O87" s="1"/>
+      <c r="P87" s="1"/>
+    </row>
+    <row r="88" spans="1:16">
       <c r="A88" t="s">
         <v>14</v>
       </c>
@@ -2553,14 +3234,22 @@
       <c r="E88">
         <v>201503</v>
       </c>
-      <c r="F88" s="1">
+      <c r="F88">
+        <f t="shared" si="2"/>
+        <v>24.499999999999996</v>
+      </c>
+      <c r="G88" s="1">
         <v>76.099999999999994</v>
       </c>
-      <c r="G88" s="1">
+      <c r="H88" s="1">
+        <f t="shared" si="3"/>
+        <v>45.211999999999996</v>
+      </c>
+      <c r="I88" s="1">
         <v>1.78</v>
       </c>
     </row>
-    <row r="89" spans="1:14">
+    <row r="89" spans="1:16">
       <c r="A89" t="s">
         <v>14</v>
       </c>
@@ -2576,14 +3265,22 @@
       <c r="E89">
         <v>201504</v>
       </c>
-      <c r="F89" s="1">
+      <c r="F89">
+        <f t="shared" si="2"/>
+        <v>26</v>
+      </c>
+      <c r="G89" s="1">
         <v>78.8</v>
       </c>
-      <c r="G89" s="1">
+      <c r="H89" s="1">
+        <f t="shared" si="3"/>
+        <v>15.747999999999999</v>
+      </c>
+      <c r="I89" s="1">
         <v>0.62</v>
       </c>
     </row>
-    <row r="90" spans="1:14">
+    <row r="90" spans="1:16">
       <c r="A90" t="s">
         <v>14</v>
       </c>
@@ -2599,14 +3296,22 @@
       <c r="E90">
         <v>201505</v>
       </c>
-      <c r="F90" s="1">
+      <c r="F90">
+        <f t="shared" si="2"/>
+        <v>27.333333333333332</v>
+      </c>
+      <c r="G90" s="1">
         <v>81.2</v>
       </c>
-      <c r="G90" s="1">
+      <c r="H90" s="1">
+        <f t="shared" si="3"/>
+        <v>25.654</v>
+      </c>
+      <c r="I90" s="1">
         <v>1.01</v>
       </c>
     </row>
-    <row r="91" spans="1:14">
+    <row r="91" spans="1:16">
       <c r="A91" t="s">
         <v>14</v>
       </c>
@@ -2622,14 +3327,22 @@
       <c r="E91">
         <v>201506</v>
       </c>
-      <c r="F91" s="1">
+      <c r="F91">
+        <f t="shared" si="2"/>
+        <v>28.166666666666668</v>
+      </c>
+      <c r="G91" s="1">
         <v>82.7</v>
       </c>
-      <c r="G91" s="1">
+      <c r="H91" s="1">
+        <f t="shared" si="3"/>
+        <v>31.75</v>
+      </c>
+      <c r="I91" s="1">
         <v>1.25</v>
       </c>
     </row>
-    <row r="92" spans="1:14">
+    <row r="92" spans="1:16">
       <c r="A92" t="s">
         <v>14</v>
       </c>
@@ -2645,20 +3358,28 @@
       <c r="E92">
         <v>201507</v>
       </c>
-      <c r="F92" s="1">
+      <c r="F92">
+        <f t="shared" si="2"/>
+        <v>28.055555555555557</v>
+      </c>
+      <c r="G92" s="1">
         <v>82.5</v>
       </c>
-      <c r="G92" s="1">
+      <c r="H92" s="1">
+        <f t="shared" si="3"/>
+        <v>37.591999999999999</v>
+      </c>
+      <c r="I92" s="1">
         <v>1.48</v>
       </c>
-      <c r="H92" s="1"/>
-      <c r="I92" s="1"/>
       <c r="J92" s="1"/>
       <c r="K92" s="1"/>
       <c r="L92" s="1"/>
       <c r="M92" s="1"/>
-    </row>
-    <row r="93" spans="1:14">
+      <c r="N92" s="1"/>
+      <c r="O92" s="1"/>
+    </row>
+    <row r="93" spans="1:16">
       <c r="A93" t="s">
         <v>14</v>
       </c>
@@ -2674,14 +3395,22 @@
       <c r="E93">
         <v>201508</v>
       </c>
-      <c r="F93" s="1">
+      <c r="F93">
+        <f t="shared" si="2"/>
+        <v>28.166666666666668</v>
+      </c>
+      <c r="G93" s="1">
         <v>82.7</v>
       </c>
-      <c r="G93" s="1">
+      <c r="H93" s="1">
+        <f t="shared" si="3"/>
+        <v>115.31599999999999</v>
+      </c>
+      <c r="I93" s="1">
         <v>4.54</v>
       </c>
     </row>
-    <row r="94" spans="1:14">
+    <row r="94" spans="1:16">
       <c r="A94" t="s">
         <v>14</v>
       </c>
@@ -2697,14 +3426,22 @@
       <c r="E94">
         <v>201509</v>
       </c>
-      <c r="F94" s="1">
+      <c r="F94">
+        <f t="shared" si="2"/>
+        <v>28.333333333333332</v>
+      </c>
+      <c r="G94" s="1">
         <v>83</v>
       </c>
-      <c r="G94" s="1">
+      <c r="H94" s="1">
+        <f t="shared" si="3"/>
+        <v>54.609999999999992</v>
+      </c>
+      <c r="I94" s="1">
         <v>2.15</v>
       </c>
     </row>
-    <row r="95" spans="1:14">
+    <row r="95" spans="1:16">
       <c r="A95" t="s">
         <v>14</v>
       </c>
@@ -2720,14 +3457,22 @@
       <c r="E95">
         <v>201510</v>
       </c>
-      <c r="F95" s="1">
+      <c r="F95">
+        <f t="shared" si="2"/>
+        <v>27.722222222222225</v>
+      </c>
+      <c r="G95" s="1">
         <v>81.900000000000006</v>
       </c>
-      <c r="G95" s="1">
+      <c r="H95" s="1">
+        <f t="shared" si="3"/>
+        <v>242.06199999999998</v>
+      </c>
+      <c r="I95" s="1">
         <v>9.5299999999999994</v>
       </c>
     </row>
-    <row r="96" spans="1:14">
+    <row r="96" spans="1:16">
       <c r="A96" t="s">
         <v>14</v>
       </c>
@@ -2743,14 +3488,22 @@
       <c r="E96">
         <v>201511</v>
       </c>
-      <c r="F96" s="1">
+      <c r="F96">
+        <f t="shared" si="2"/>
+        <v>26.222222222222221</v>
+      </c>
+      <c r="G96" s="1">
         <v>79.2</v>
       </c>
-      <c r="G96" s="1">
+      <c r="H96" s="1">
+        <f t="shared" si="3"/>
+        <v>239.52199999999999</v>
+      </c>
+      <c r="I96" s="1">
         <v>9.43</v>
       </c>
     </row>
-    <row r="97" spans="1:15">
+    <row r="97" spans="1:17">
       <c r="A97" t="s">
         <v>14</v>
       </c>
@@ -2766,14 +3519,22 @@
       <c r="E97">
         <v>201512</v>
       </c>
-      <c r="F97" s="1">
+      <c r="F97">
+        <f t="shared" si="2"/>
+        <v>25.277777777777779</v>
+      </c>
+      <c r="G97" s="1">
         <v>77.5</v>
       </c>
-      <c r="G97" s="1">
+      <c r="H97" s="1">
+        <f t="shared" si="3"/>
+        <v>176.02199999999999</v>
+      </c>
+      <c r="I97" s="1">
         <v>6.93</v>
       </c>
     </row>
-    <row r="98" spans="1:15">
+    <row r="98" spans="1:17">
       <c r="A98" t="s">
         <v>15</v>
       </c>
@@ -2789,14 +3550,21 @@
       <c r="E98">
         <v>201501</v>
       </c>
-      <c r="F98" s="1">
+      <c r="F98">
+        <f t="shared" si="2"/>
+        <v>24.388888888888893</v>
+      </c>
+      <c r="G98" s="1">
         <v>75.900000000000006</v>
       </c>
-      <c r="G98" s="1">
-        <v>-9999</v>
-      </c>
-    </row>
-    <row r="99" spans="1:15">
+      <c r="H98" s="1">
+        <v>-9999</v>
+      </c>
+      <c r="I98" s="1">
+        <v>-9999</v>
+      </c>
+    </row>
+    <row r="99" spans="1:17">
       <c r="A99" t="s">
         <v>15</v>
       </c>
@@ -2812,22 +3580,30 @@
       <c r="E99">
         <v>201502</v>
       </c>
-      <c r="F99" s="1">
+      <c r="F99">
+        <f t="shared" si="2"/>
+        <v>24.611111111111111</v>
+      </c>
+      <c r="G99" s="1">
         <v>76.3</v>
       </c>
-      <c r="G99" s="1">
+      <c r="H99" s="1">
+        <f t="shared" si="3"/>
+        <v>85.597999999999999</v>
+      </c>
+      <c r="I99" s="1">
         <v>3.37</v>
       </c>
-      <c r="H99" s="1"/>
-      <c r="I99" s="1"/>
       <c r="J99" s="1"/>
       <c r="K99" s="1"/>
       <c r="L99" s="1"/>
       <c r="M99" s="1"/>
       <c r="N99" s="1"/>
       <c r="O99" s="1"/>
-    </row>
-    <row r="100" spans="1:15">
+      <c r="P99" s="1"/>
+      <c r="Q99" s="1"/>
+    </row>
+    <row r="100" spans="1:17">
       <c r="A100" t="s">
         <v>15</v>
       </c>
@@ -2843,20 +3619,27 @@
       <c r="E100">
         <v>201503</v>
       </c>
-      <c r="F100" s="1">
+      <c r="F100">
+        <f t="shared" si="2"/>
+        <v>23.888888888888889</v>
+      </c>
+      <c r="G100" s="1">
         <v>75</v>
       </c>
-      <c r="G100" s="1">
-        <v>-9999</v>
-      </c>
-      <c r="H100" s="1"/>
-      <c r="I100" s="1"/>
+      <c r="H100" s="1">
+        <v>-9999</v>
+      </c>
+      <c r="I100" s="1">
+        <v>-9999</v>
+      </c>
       <c r="J100" s="1"/>
       <c r="K100" s="1"/>
       <c r="L100" s="1"/>
       <c r="M100" s="1"/>
-    </row>
-    <row r="101" spans="1:15">
+      <c r="N100" s="1"/>
+      <c r="O100" s="1"/>
+    </row>
+    <row r="101" spans="1:17">
       <c r="A101" t="s">
         <v>15</v>
       </c>
@@ -2872,14 +3655,21 @@
       <c r="E101">
         <v>201504</v>
       </c>
-      <c r="F101" s="1">
+      <c r="F101">
+        <f t="shared" si="2"/>
+        <v>24.833333333333332</v>
+      </c>
+      <c r="G101" s="1">
         <v>76.7</v>
       </c>
-      <c r="G101" s="1">
-        <v>-9999</v>
-      </c>
-    </row>
-    <row r="102" spans="1:15">
+      <c r="H101" s="1">
+        <v>-9999</v>
+      </c>
+      <c r="I101" s="1">
+        <v>-9999</v>
+      </c>
+    </row>
+    <row r="102" spans="1:17">
       <c r="A102" t="s">
         <v>15</v>
       </c>
@@ -2895,14 +3685,22 @@
       <c r="E102">
         <v>201505</v>
       </c>
-      <c r="F102" s="1">
+      <c r="F102">
+        <f t="shared" si="2"/>
+        <v>26.166666666666664</v>
+      </c>
+      <c r="G102" s="1">
         <v>79.099999999999994</v>
       </c>
-      <c r="G102" s="1">
+      <c r="H102" s="1">
+        <f t="shared" si="3"/>
+        <v>108.712</v>
+      </c>
+      <c r="I102" s="1">
         <v>4.28</v>
       </c>
     </row>
-    <row r="103" spans="1:15">
+    <row r="103" spans="1:17">
       <c r="A103" t="s">
         <v>15</v>
       </c>
@@ -2918,14 +3716,21 @@
       <c r="E103">
         <v>201506</v>
       </c>
-      <c r="F103" s="1">
+      <c r="F103">
+        <f t="shared" si="2"/>
+        <v>27.444444444444446</v>
+      </c>
+      <c r="G103" s="1">
         <v>81.400000000000006</v>
       </c>
-      <c r="G103" s="1">
-        <v>-9999</v>
-      </c>
-    </row>
-    <row r="104" spans="1:15">
+      <c r="H103" s="1">
+        <v>-9999</v>
+      </c>
+      <c r="I103" s="1">
+        <v>-9999</v>
+      </c>
+    </row>
+    <row r="104" spans="1:17">
       <c r="A104" t="s">
         <v>15</v>
       </c>
@@ -2941,14 +3746,21 @@
       <c r="E104">
         <v>201507</v>
       </c>
-      <c r="F104" s="1">
+      <c r="F104">
+        <f t="shared" si="2"/>
+        <v>27.444444444444446</v>
+      </c>
+      <c r="G104" s="1">
         <v>81.400000000000006</v>
       </c>
-      <c r="G104" s="1">
-        <v>-9999</v>
-      </c>
-    </row>
-    <row r="105" spans="1:15">
+      <c r="H104" s="1">
+        <v>-9999</v>
+      </c>
+      <c r="I104" s="1">
+        <v>-9999</v>
+      </c>
+    </row>
+    <row r="105" spans="1:17">
       <c r="A105" t="s">
         <v>15</v>
       </c>
@@ -2964,14 +3776,22 @@
       <c r="E105">
         <v>201508</v>
       </c>
-      <c r="F105" s="1">
+      <c r="F105">
+        <f t="shared" si="2"/>
+        <v>27.333333333333332</v>
+      </c>
+      <c r="G105" s="1">
         <v>81.2</v>
       </c>
-      <c r="G105" s="1">
+      <c r="H105" s="1">
+        <f t="shared" si="3"/>
+        <v>65.024000000000001</v>
+      </c>
+      <c r="I105" s="1">
         <v>2.56</v>
       </c>
     </row>
-    <row r="106" spans="1:15">
+    <row r="106" spans="1:17">
       <c r="A106" t="s">
         <v>15</v>
       </c>
@@ -2987,19 +3807,27 @@
       <c r="E106">
         <v>201509</v>
       </c>
-      <c r="F106" s="1">
+      <c r="F106">
+        <f t="shared" si="2"/>
+        <v>27.777777777777779</v>
+      </c>
+      <c r="G106" s="1">
         <v>82</v>
       </c>
-      <c r="G106" s="1">
+      <c r="H106" s="1">
+        <f t="shared" si="3"/>
+        <v>74.421999999999997</v>
+      </c>
+      <c r="I106" s="1">
         <v>2.93</v>
       </c>
-      <c r="H106" s="1"/>
-      <c r="I106" s="1"/>
       <c r="J106" s="1"/>
       <c r="K106" s="1"/>
       <c r="L106" s="1"/>
-    </row>
-    <row r="107" spans="1:15">
+      <c r="M106" s="1"/>
+      <c r="N106" s="1"/>
+    </row>
+    <row r="107" spans="1:17">
       <c r="A107" t="s">
         <v>15</v>
       </c>
@@ -3015,14 +3843,21 @@
       <c r="E107">
         <v>201510</v>
       </c>
-      <c r="F107" s="1">
+      <c r="F107">
+        <f t="shared" si="2"/>
+        <v>27.833333333333329</v>
+      </c>
+      <c r="G107" s="1">
         <v>82.1</v>
       </c>
-      <c r="G107" s="1">
-        <v>-9999</v>
-      </c>
-    </row>
-    <row r="108" spans="1:15">
+      <c r="H107" s="1">
+        <v>-9999</v>
+      </c>
+      <c r="I107" s="1">
+        <v>-9999</v>
+      </c>
+    </row>
+    <row r="108" spans="1:17">
       <c r="A108" t="s">
         <v>15</v>
       </c>
@@ -3044,8 +3879,14 @@
       <c r="G108" s="1">
         <v>-9999</v>
       </c>
-    </row>
-    <row r="109" spans="1:15">
+      <c r="H108" s="1">
+        <v>-9999</v>
+      </c>
+      <c r="I108" s="1">
+        <v>-9999</v>
+      </c>
+    </row>
+    <row r="109" spans="1:17">
       <c r="A109" t="s">
         <v>15</v>
       </c>
@@ -3067,8 +3908,14 @@
       <c r="G109" s="1">
         <v>-9999</v>
       </c>
-    </row>
-    <row r="110" spans="1:15">
+      <c r="H109" s="1">
+        <v>-9999</v>
+      </c>
+      <c r="I109" s="1">
+        <v>-9999</v>
+      </c>
+    </row>
+    <row r="110" spans="1:17">
       <c r="A110" t="s">
         <v>16</v>
       </c>
@@ -3088,10 +3935,17 @@
         <v>-9999</v>
       </c>
       <c r="G110" s="1">
+        <v>-9999</v>
+      </c>
+      <c r="H110" s="1">
+        <f t="shared" si="3"/>
+        <v>57.403999999999989</v>
+      </c>
+      <c r="I110" s="1">
         <v>2.2599999999999998</v>
       </c>
     </row>
-    <row r="111" spans="1:15">
+    <row r="111" spans="1:17">
       <c r="A111" t="s">
         <v>16</v>
       </c>
@@ -3111,15 +3965,22 @@
         <v>-9999</v>
       </c>
       <c r="G111" s="1">
+        <v>-9999</v>
+      </c>
+      <c r="H111" s="1">
+        <f t="shared" si="3"/>
+        <v>88.138000000000005</v>
+      </c>
+      <c r="I111" s="1">
         <v>3.47</v>
       </c>
-      <c r="H111" s="1"/>
-      <c r="I111" s="1"/>
       <c r="J111" s="1"/>
       <c r="K111" s="1"/>
       <c r="L111" s="1"/>
-    </row>
-    <row r="112" spans="1:15">
+      <c r="M111" s="1"/>
+      <c r="N111" s="1"/>
+    </row>
+    <row r="112" spans="1:17">
       <c r="A112" t="s">
         <v>16</v>
       </c>
@@ -3139,15 +4000,22 @@
         <v>-9999</v>
       </c>
       <c r="G112" s="1">
+        <v>-9999</v>
+      </c>
+      <c r="H112" s="1">
+        <f t="shared" si="3"/>
+        <v>85.343999999999994</v>
+      </c>
+      <c r="I112" s="1">
         <v>3.36</v>
       </c>
-      <c r="H112" s="1"/>
-      <c r="I112" s="1"/>
       <c r="J112" s="1"/>
       <c r="K112" s="1"/>
       <c r="L112" s="1"/>
-    </row>
-    <row r="113" spans="1:12">
+      <c r="M112" s="1"/>
+      <c r="N112" s="1"/>
+    </row>
+    <row r="113" spans="1:14">
       <c r="A113" t="s">
         <v>16</v>
       </c>
@@ -3167,10 +4035,17 @@
         <v>-9999</v>
       </c>
       <c r="G113" s="1">
+        <v>-9999</v>
+      </c>
+      <c r="H113" s="1">
+        <f t="shared" si="3"/>
+        <v>34.544000000000004</v>
+      </c>
+      <c r="I113" s="1">
         <v>1.36</v>
       </c>
     </row>
-    <row r="114" spans="1:12">
+    <row r="114" spans="1:14">
       <c r="A114" t="s">
         <v>16</v>
       </c>
@@ -3190,10 +4065,17 @@
         <v>-9999</v>
       </c>
       <c r="G114" s="1">
+        <v>-9999</v>
+      </c>
+      <c r="H114" s="1">
+        <f t="shared" si="3"/>
+        <v>182.37199999999999</v>
+      </c>
+      <c r="I114" s="1">
         <v>7.18</v>
       </c>
     </row>
-    <row r="115" spans="1:12">
+    <row r="115" spans="1:14">
       <c r="A115" t="s">
         <v>16</v>
       </c>
@@ -3213,10 +4095,17 @@
         <v>-9999</v>
       </c>
       <c r="G115" s="1">
+        <v>-9999</v>
+      </c>
+      <c r="H115" s="1">
+        <f t="shared" si="3"/>
+        <v>92.71</v>
+      </c>
+      <c r="I115" s="1">
         <v>3.65</v>
       </c>
     </row>
-    <row r="116" spans="1:12">
+    <row r="116" spans="1:14">
       <c r="A116" t="s">
         <v>16</v>
       </c>
@@ -3236,10 +4125,17 @@
         <v>-9999</v>
       </c>
       <c r="G116" s="1">
+        <v>-9999</v>
+      </c>
+      <c r="H116" s="1">
+        <f t="shared" si="3"/>
+        <v>16.001999999999999</v>
+      </c>
+      <c r="I116" s="1">
         <v>0.63</v>
       </c>
     </row>
-    <row r="117" spans="1:12">
+    <row r="117" spans="1:14">
       <c r="A117" t="s">
         <v>16</v>
       </c>
@@ -3259,10 +4155,17 @@
         <v>-9999</v>
       </c>
       <c r="G117" s="1">
+        <v>-9999</v>
+      </c>
+      <c r="H117" s="1">
+        <f t="shared" si="3"/>
+        <v>200.66</v>
+      </c>
+      <c r="I117" s="1">
         <v>7.9</v>
       </c>
     </row>
-    <row r="118" spans="1:12">
+    <row r="118" spans="1:14">
       <c r="A118" t="s">
         <v>16</v>
       </c>
@@ -3282,10 +4185,17 @@
         <v>-9999</v>
       </c>
       <c r="G118" s="1">
+        <v>-9999</v>
+      </c>
+      <c r="H118" s="1">
+        <f t="shared" si="3"/>
+        <v>339.09</v>
+      </c>
+      <c r="I118" s="1">
         <v>13.35</v>
       </c>
     </row>
-    <row r="119" spans="1:12">
+    <row r="119" spans="1:14">
       <c r="A119" t="s">
         <v>16</v>
       </c>
@@ -3305,10 +4215,17 @@
         <v>-9999</v>
       </c>
       <c r="G119" s="1">
+        <v>-9999</v>
+      </c>
+      <c r="H119" s="1">
+        <f t="shared" si="3"/>
+        <v>135.12799999999999</v>
+      </c>
+      <c r="I119" s="1">
         <v>5.32</v>
       </c>
     </row>
-    <row r="120" spans="1:12">
+    <row r="120" spans="1:14">
       <c r="A120" t="s">
         <v>16</v>
       </c>
@@ -3328,10 +4245,17 @@
         <v>-9999</v>
       </c>
       <c r="G120" s="1">
+        <v>-9999</v>
+      </c>
+      <c r="H120" s="1">
+        <f t="shared" si="3"/>
+        <v>261.11199999999997</v>
+      </c>
+      <c r="I120" s="1">
         <v>10.28</v>
       </c>
     </row>
-    <row r="121" spans="1:12">
+    <row r="121" spans="1:14">
       <c r="A121" t="s">
         <v>16</v>
       </c>
@@ -3351,10 +4275,17 @@
         <v>-9999</v>
       </c>
       <c r="G121" s="1">
+        <v>-9999</v>
+      </c>
+      <c r="H121" s="1">
+        <f t="shared" si="3"/>
+        <v>39.116</v>
+      </c>
+      <c r="I121" s="1">
         <v>1.54</v>
       </c>
     </row>
-    <row r="122" spans="1:12">
+    <row r="122" spans="1:14">
       <c r="A122" t="s">
         <v>17</v>
       </c>
@@ -3370,19 +4301,27 @@
       <c r="E122">
         <v>201501</v>
       </c>
-      <c r="F122" s="1">
+      <c r="F122">
+        <f t="shared" si="2"/>
+        <v>21.999999999999996</v>
+      </c>
+      <c r="G122" s="1">
         <v>71.599999999999994</v>
       </c>
-      <c r="G122" s="1">
+      <c r="H122" s="1">
+        <f t="shared" si="3"/>
+        <v>162.81399999999999</v>
+      </c>
+      <c r="I122" s="1">
         <v>6.41</v>
       </c>
-      <c r="H122" s="1"/>
-      <c r="I122" s="1"/>
       <c r="J122" s="1"/>
       <c r="K122" s="1"/>
       <c r="L122" s="1"/>
-    </row>
-    <row r="123" spans="1:12">
+      <c r="M122" s="1"/>
+      <c r="N122" s="1"/>
+    </row>
+    <row r="123" spans="1:14">
       <c r="A123" t="s">
         <v>17</v>
       </c>
@@ -3398,14 +4337,22 @@
       <c r="E123">
         <v>201502</v>
       </c>
-      <c r="F123" s="1">
+      <c r="F123">
+        <f t="shared" si="2"/>
+        <v>22.111111111111111</v>
+      </c>
+      <c r="G123" s="1">
         <v>71.8</v>
       </c>
-      <c r="G123" s="1">
+      <c r="H123" s="1">
+        <f t="shared" si="3"/>
+        <v>192.02399999999997</v>
+      </c>
+      <c r="I123" s="1">
         <v>7.56</v>
       </c>
     </row>
-    <row r="124" spans="1:12">
+    <row r="124" spans="1:14">
       <c r="A124" t="s">
         <v>17</v>
       </c>
@@ -3421,14 +4368,22 @@
       <c r="E124">
         <v>201503</v>
       </c>
-      <c r="F124" s="1">
+      <c r="F124">
+        <f t="shared" si="2"/>
+        <v>21.944444444444443</v>
+      </c>
+      <c r="G124" s="1">
         <v>71.5</v>
       </c>
-      <c r="G124" s="1">
+      <c r="H124" s="1">
+        <f t="shared" si="3"/>
+        <v>90.169999999999987</v>
+      </c>
+      <c r="I124" s="1">
         <v>3.55</v>
       </c>
     </row>
-    <row r="125" spans="1:12">
+    <row r="125" spans="1:14">
       <c r="A125" t="s">
         <v>17</v>
       </c>
@@ -3444,14 +4399,22 @@
       <c r="E125">
         <v>201504</v>
       </c>
-      <c r="F125" s="1">
+      <c r="F125">
+        <f t="shared" si="2"/>
+        <v>23.222222222222221</v>
+      </c>
+      <c r="G125" s="1">
         <v>73.8</v>
       </c>
-      <c r="G125" s="1">
+      <c r="H125" s="1">
+        <f t="shared" si="3"/>
+        <v>46.99</v>
+      </c>
+      <c r="I125" s="1">
         <v>1.85</v>
       </c>
     </row>
-    <row r="126" spans="1:12">
+    <row r="126" spans="1:14">
       <c r="A126" t="s">
         <v>17</v>
       </c>
@@ -3467,14 +4430,22 @@
       <c r="E126">
         <v>201505</v>
       </c>
-      <c r="F126" s="1">
+      <c r="F126">
+        <f t="shared" si="2"/>
+        <v>24.277777777777779</v>
+      </c>
+      <c r="G126" s="1">
         <v>75.7</v>
       </c>
-      <c r="G126" s="1">
+      <c r="H126" s="1">
+        <f t="shared" si="3"/>
+        <v>91.44</v>
+      </c>
+      <c r="I126" s="1">
         <v>3.6</v>
       </c>
     </row>
-    <row r="127" spans="1:12">
+    <row r="127" spans="1:14">
       <c r="A127" t="s">
         <v>17</v>
       </c>
@@ -3490,14 +4461,22 @@
       <c r="E127">
         <v>201506</v>
       </c>
-      <c r="F127" s="1">
+      <c r="F127">
+        <f t="shared" si="2"/>
+        <v>25.055555555555554</v>
+      </c>
+      <c r="G127" s="1">
         <v>77.099999999999994</v>
       </c>
-      <c r="G127" s="1">
+      <c r="H127" s="1">
+        <f t="shared" si="3"/>
+        <v>54.863999999999997</v>
+      </c>
+      <c r="I127" s="1">
         <v>2.16</v>
       </c>
     </row>
-    <row r="128" spans="1:12">
+    <row r="128" spans="1:14">
       <c r="A128" t="s">
         <v>17</v>
       </c>
@@ -3513,14 +4492,22 @@
       <c r="E128">
         <v>201507</v>
       </c>
-      <c r="F128" s="1">
+      <c r="F128">
+        <f t="shared" si="2"/>
+        <v>24.888888888888889</v>
+      </c>
+      <c r="G128" s="1">
         <v>76.8</v>
       </c>
-      <c r="G128" s="1">
+      <c r="H128" s="1">
+        <f t="shared" si="3"/>
+        <v>46.735999999999997</v>
+      </c>
+      <c r="I128" s="1">
         <v>1.84</v>
       </c>
     </row>
-    <row r="129" spans="1:12">
+    <row r="129" spans="1:14">
       <c r="A129" t="s">
         <v>17</v>
       </c>
@@ -3536,14 +4523,22 @@
       <c r="E129">
         <v>201508</v>
       </c>
-      <c r="F129" s="1">
+      <c r="F129">
+        <f t="shared" si="2"/>
+        <v>25.277777777777779</v>
+      </c>
+      <c r="G129" s="1">
         <v>77.5</v>
       </c>
-      <c r="G129" s="1">
+      <c r="H129" s="1">
+        <f t="shared" si="3"/>
+        <v>179.578</v>
+      </c>
+      <c r="I129" s="1">
         <v>7.07</v>
       </c>
     </row>
-    <row r="130" spans="1:12">
+    <row r="130" spans="1:14">
       <c r="A130" t="s">
         <v>17</v>
       </c>
@@ -3559,14 +4554,22 @@
       <c r="E130">
         <v>201509</v>
       </c>
-      <c r="F130" s="1">
+      <c r="F130">
+        <f t="shared" si="2"/>
+        <v>25.555555555555557</v>
+      </c>
+      <c r="G130" s="1">
         <v>78</v>
       </c>
-      <c r="G130" s="1">
+      <c r="H130" s="1">
+        <f t="shared" si="3"/>
+        <v>127.25399999999999</v>
+      </c>
+      <c r="I130" s="1">
         <v>5.01</v>
       </c>
     </row>
-    <row r="131" spans="1:12">
+    <row r="131" spans="1:14">
       <c r="A131" t="s">
         <v>17</v>
       </c>
@@ -3582,14 +4585,22 @@
       <c r="E131">
         <v>201510</v>
       </c>
-      <c r="F131" s="1">
+      <c r="F131">
+        <f t="shared" ref="F131:F181" si="4">(G131-32)*5/9</f>
+        <v>25.333333333333329</v>
+      </c>
+      <c r="G131" s="1">
         <v>77.599999999999994</v>
       </c>
-      <c r="G131" s="1">
+      <c r="H131" s="1">
+        <f t="shared" ref="H131:H181" si="5">I131*25.4</f>
+        <v>132.07999999999998</v>
+      </c>
+      <c r="I131" s="1">
         <v>5.2</v>
       </c>
     </row>
-    <row r="132" spans="1:12">
+    <row r="132" spans="1:14">
       <c r="A132" t="s">
         <v>17</v>
       </c>
@@ -3605,14 +4616,22 @@
       <c r="E132">
         <v>201511</v>
       </c>
-      <c r="F132" s="1">
+      <c r="F132">
+        <f t="shared" si="4"/>
+        <v>23.666666666666664</v>
+      </c>
+      <c r="G132" s="1">
         <v>74.599999999999994</v>
       </c>
-      <c r="G132" s="1">
+      <c r="H132" s="1">
+        <f t="shared" si="5"/>
+        <v>234.696</v>
+      </c>
+      <c r="I132" s="1">
         <v>9.24</v>
       </c>
     </row>
-    <row r="133" spans="1:12">
+    <row r="133" spans="1:14">
       <c r="A133" t="s">
         <v>17</v>
       </c>
@@ -3628,14 +4647,22 @@
       <c r="E133">
         <v>201512</v>
       </c>
-      <c r="F133" s="1">
+      <c r="F133">
+        <f t="shared" si="4"/>
+        <v>22.722222222222225</v>
+      </c>
+      <c r="G133" s="1">
         <v>72.900000000000006</v>
       </c>
-      <c r="G133" s="1">
+      <c r="H133" s="1">
+        <f t="shared" si="5"/>
+        <v>163.32199999999997</v>
+      </c>
+      <c r="I133" s="1">
         <v>6.43</v>
       </c>
     </row>
-    <row r="134" spans="1:12">
+    <row r="134" spans="1:14">
       <c r="A134" t="s">
         <v>18</v>
       </c>
@@ -3651,14 +4678,22 @@
       <c r="E134">
         <v>201501</v>
       </c>
-      <c r="F134" s="1">
+      <c r="F134">
+        <f t="shared" si="4"/>
+        <v>23.444444444444443</v>
+      </c>
+      <c r="G134" s="1">
         <v>74.2</v>
       </c>
-      <c r="G134" s="1">
+      <c r="H134" s="1">
+        <f t="shared" si="5"/>
+        <v>58.92799999999999</v>
+      </c>
+      <c r="I134" s="1">
         <v>2.3199999999999998</v>
       </c>
     </row>
-    <row r="135" spans="1:12">
+    <row r="135" spans="1:14">
       <c r="A135" t="s">
         <v>18</v>
       </c>
@@ -3674,14 +4709,22 @@
       <c r="E135">
         <v>201502</v>
       </c>
-      <c r="F135" s="1">
+      <c r="F135">
+        <f t="shared" si="4"/>
+        <v>23.555555555555557</v>
+      </c>
+      <c r="G135" s="1">
         <v>74.400000000000006</v>
       </c>
-      <c r="G135" s="1">
+      <c r="H135" s="1">
+        <f t="shared" si="5"/>
+        <v>109.47399999999999</v>
+      </c>
+      <c r="I135" s="1">
         <v>4.3099999999999996</v>
       </c>
     </row>
-    <row r="136" spans="1:12">
+    <row r="136" spans="1:14">
       <c r="A136" t="s">
         <v>18</v>
       </c>
@@ -3697,14 +4740,22 @@
       <c r="E136">
         <v>201503</v>
       </c>
-      <c r="F136" s="1">
+      <c r="F136">
+        <f t="shared" si="4"/>
+        <v>23.055555555555557</v>
+      </c>
+      <c r="G136" s="1">
         <v>73.5</v>
       </c>
-      <c r="G136" s="1">
+      <c r="H136" s="1">
+        <f t="shared" si="5"/>
+        <v>82.296000000000006</v>
+      </c>
+      <c r="I136" s="1">
         <v>3.24</v>
       </c>
     </row>
-    <row r="137" spans="1:12">
+    <row r="137" spans="1:14">
       <c r="A137" t="s">
         <v>18</v>
       </c>
@@ -3720,14 +4771,22 @@
       <c r="E137">
         <v>201504</v>
       </c>
-      <c r="F137" s="1">
+      <c r="F137">
+        <f t="shared" si="4"/>
+        <v>24.222222222222218</v>
+      </c>
+      <c r="G137" s="1">
         <v>75.599999999999994</v>
       </c>
-      <c r="G137" s="1">
+      <c r="H137" s="1">
+        <f t="shared" si="5"/>
+        <v>58.673999999999999</v>
+      </c>
+      <c r="I137" s="1">
         <v>2.31</v>
       </c>
     </row>
-    <row r="138" spans="1:12">
+    <row r="138" spans="1:14">
       <c r="A138" t="s">
         <v>18</v>
       </c>
@@ -3743,19 +4802,27 @@
       <c r="E138">
         <v>201505</v>
       </c>
-      <c r="F138" s="1">
+      <c r="F138">
+        <f t="shared" si="4"/>
+        <v>25.777777777777782</v>
+      </c>
+      <c r="G138" s="1">
         <v>78.400000000000006</v>
       </c>
-      <c r="G138" s="1">
+      <c r="H138" s="1">
+        <f t="shared" si="5"/>
+        <v>98.551999999999992</v>
+      </c>
+      <c r="I138" s="1">
         <v>3.88</v>
       </c>
-      <c r="H138" s="1"/>
-      <c r="I138" s="1"/>
       <c r="J138" s="1"/>
       <c r="K138" s="1"/>
       <c r="L138" s="1"/>
-    </row>
-    <row r="139" spans="1:12">
+      <c r="M138" s="1"/>
+      <c r="N138" s="1"/>
+    </row>
+    <row r="139" spans="1:14">
       <c r="A139" t="s">
         <v>18</v>
       </c>
@@ -3771,14 +4838,22 @@
       <c r="E139">
         <v>201506</v>
       </c>
-      <c r="F139" s="1">
+      <c r="F139">
+        <f t="shared" si="4"/>
+        <v>26.333333333333336</v>
+      </c>
+      <c r="G139" s="1">
         <v>79.400000000000006</v>
       </c>
-      <c r="G139" s="1">
+      <c r="H139" s="1">
+        <f t="shared" si="5"/>
+        <v>118.11</v>
+      </c>
+      <c r="I139" s="1">
         <v>4.6500000000000004</v>
       </c>
     </row>
-    <row r="140" spans="1:12">
+    <row r="140" spans="1:14">
       <c r="A140" t="s">
         <v>18</v>
       </c>
@@ -3794,14 +4869,22 @@
       <c r="E140">
         <v>201507</v>
       </c>
-      <c r="F140" s="1">
+      <c r="F140">
+        <f t="shared" si="4"/>
+        <v>26.5</v>
+      </c>
+      <c r="G140" s="1">
         <v>79.7</v>
       </c>
-      <c r="G140" s="1">
+      <c r="H140" s="1">
+        <f t="shared" si="5"/>
+        <v>32.765999999999998</v>
+      </c>
+      <c r="I140" s="1">
         <v>1.29</v>
       </c>
     </row>
-    <row r="141" spans="1:12">
+    <row r="141" spans="1:14">
       <c r="A141" t="s">
         <v>18</v>
       </c>
@@ -3817,14 +4900,22 @@
       <c r="E141">
         <v>201508</v>
       </c>
-      <c r="F141" s="1">
+      <c r="F141">
+        <f t="shared" si="4"/>
+        <v>26.666666666666668</v>
+      </c>
+      <c r="G141" s="1">
         <v>80</v>
       </c>
-      <c r="G141" s="1">
+      <c r="H141" s="1">
+        <f t="shared" si="5"/>
+        <v>104.648</v>
+      </c>
+      <c r="I141" s="1">
         <v>4.12</v>
       </c>
     </row>
-    <row r="142" spans="1:12">
+    <row r="142" spans="1:14">
       <c r="A142" t="s">
         <v>18</v>
       </c>
@@ -3840,14 +4931,22 @@
       <c r="E142">
         <v>201509</v>
       </c>
-      <c r="F142" s="1">
+      <c r="F142">
+        <f t="shared" si="4"/>
+        <v>26.611111111111114</v>
+      </c>
+      <c r="G142" s="1">
         <v>79.900000000000006</v>
       </c>
-      <c r="G142" s="1">
+      <c r="H142" s="1">
+        <f t="shared" si="5"/>
+        <v>234.18800000000002</v>
+      </c>
+      <c r="I142" s="1">
         <v>9.2200000000000006</v>
       </c>
     </row>
-    <row r="143" spans="1:12">
+    <row r="143" spans="1:14">
       <c r="A143" t="s">
         <v>18</v>
       </c>
@@ -3863,14 +4962,22 @@
       <c r="E143">
         <v>201510</v>
       </c>
-      <c r="F143" s="1">
+      <c r="F143">
+        <f t="shared" si="4"/>
+        <v>26.555555555555557</v>
+      </c>
+      <c r="G143" s="1">
         <v>79.8</v>
       </c>
-      <c r="G143" s="1">
+      <c r="H143" s="1">
+        <f t="shared" si="5"/>
+        <v>191.51599999999999</v>
+      </c>
+      <c r="I143" s="1">
         <v>7.54</v>
       </c>
     </row>
-    <row r="144" spans="1:12">
+    <row r="144" spans="1:14">
       <c r="A144" t="s">
         <v>18</v>
       </c>
@@ -3886,14 +4993,22 @@
       <c r="E144">
         <v>201511</v>
       </c>
-      <c r="F144" s="1">
+      <c r="F144">
+        <f t="shared" si="4"/>
+        <v>24.888888888888889</v>
+      </c>
+      <c r="G144" s="1">
         <v>76.8</v>
       </c>
-      <c r="G144" s="1">
+      <c r="H144" s="1">
+        <f t="shared" si="5"/>
+        <v>213.10599999999999</v>
+      </c>
+      <c r="I144" s="1">
         <v>8.39</v>
       </c>
     </row>
-    <row r="145" spans="1:13">
+    <row r="145" spans="1:15">
       <c r="A145" t="s">
         <v>18</v>
       </c>
@@ -3909,14 +5024,22 @@
       <c r="E145">
         <v>201512</v>
       </c>
-      <c r="F145" s="1">
+      <c r="F145">
+        <f t="shared" si="4"/>
+        <v>24.388888888888893</v>
+      </c>
+      <c r="G145" s="1">
         <v>75.900000000000006</v>
       </c>
-      <c r="G145" s="1">
+      <c r="H145" s="1">
+        <f t="shared" si="5"/>
+        <v>48.513999999999996</v>
+      </c>
+      <c r="I145" s="1">
         <v>1.91</v>
       </c>
     </row>
-    <row r="146" spans="1:13">
+    <row r="146" spans="1:15">
       <c r="A146" t="s">
         <v>19</v>
       </c>
@@ -3932,14 +5055,22 @@
       <c r="E146">
         <v>201501</v>
       </c>
-      <c r="F146" s="1">
+      <c r="F146">
+        <f t="shared" si="4"/>
+        <v>26.055555555555557</v>
+      </c>
+      <c r="G146" s="1">
         <v>78.900000000000006</v>
       </c>
-      <c r="G146" s="1">
+      <c r="H146" s="1">
+        <f t="shared" si="5"/>
+        <v>125.98399999999999</v>
+      </c>
+      <c r="I146" s="1">
         <v>4.96</v>
       </c>
     </row>
-    <row r="147" spans="1:13">
+    <row r="147" spans="1:15">
       <c r="A147" t="s">
         <v>19</v>
       </c>
@@ -3955,26 +5086,28 @@
       <c r="E147">
         <v>201502</v>
       </c>
-      <c r="F147" s="1">
+      <c r="F147">
+        <f t="shared" si="4"/>
+        <v>26.166666666666664</v>
+      </c>
+      <c r="G147" s="1">
         <v>79.099999999999994</v>
       </c>
-      <c r="G147" s="1">
+      <c r="H147" s="1">
+        <f t="shared" si="5"/>
+        <v>83.057999999999993</v>
+      </c>
+      <c r="I147" s="1">
         <v>3.27</v>
       </c>
-      <c r="H147" s="1"/>
-      <c r="I147" s="1"/>
-      <c r="J147" s="1">
-        <v>79.8</v>
-      </c>
-      <c r="K147" s="1">
-        <v>76.8</v>
-      </c>
-      <c r="L147" s="1">
-        <v>75.900000000000006</v>
-      </c>
+      <c r="J147" s="1"/>
+      <c r="K147" s="1"/>
+      <c r="L147" s="1"/>
       <c r="M147" s="1"/>
-    </row>
-    <row r="148" spans="1:13">
+      <c r="N147" s="1"/>
+      <c r="O147" s="1"/>
+    </row>
+    <row r="148" spans="1:15">
       <c r="A148" t="s">
         <v>19</v>
       </c>
@@ -3990,25 +5123,27 @@
       <c r="E148">
         <v>201503</v>
       </c>
-      <c r="F148" s="1">
+      <c r="F148">
+        <f t="shared" si="4"/>
+        <v>25.944444444444443</v>
+      </c>
+      <c r="G148" s="1">
         <v>78.7</v>
       </c>
-      <c r="G148" s="1">
+      <c r="H148" s="1">
+        <f t="shared" si="5"/>
+        <v>38.099999999999994</v>
+      </c>
+      <c r="I148" s="1">
         <v>1.5</v>
       </c>
-      <c r="H148" s="1"/>
-      <c r="I148" s="1"/>
-      <c r="J148" s="1">
-        <v>7.54</v>
-      </c>
-      <c r="K148" s="1">
-        <v>8.39</v>
-      </c>
-      <c r="L148" s="1">
-        <v>1.91</v>
-      </c>
-    </row>
-    <row r="149" spans="1:13">
+      <c r="J148" s="1"/>
+      <c r="K148" s="1"/>
+      <c r="L148" s="1"/>
+      <c r="M148" s="1"/>
+      <c r="N148" s="1"/>
+    </row>
+    <row r="149" spans="1:15">
       <c r="A149" t="s">
         <v>19</v>
       </c>
@@ -4024,14 +5159,22 @@
       <c r="E149">
         <v>201504</v>
       </c>
-      <c r="F149" s="1">
+      <c r="F149">
+        <f t="shared" si="4"/>
+        <v>27.5</v>
+      </c>
+      <c r="G149" s="1">
         <v>81.5</v>
       </c>
-      <c r="G149" s="1">
+      <c r="H149" s="1">
+        <f t="shared" si="5"/>
+        <v>35.051999999999992</v>
+      </c>
+      <c r="I149" s="1">
         <v>1.38</v>
       </c>
     </row>
-    <row r="150" spans="1:13">
+    <row r="150" spans="1:15">
       <c r="A150" t="s">
         <v>19</v>
       </c>
@@ -4047,14 +5190,22 @@
       <c r="E150">
         <v>201505</v>
       </c>
-      <c r="F150" s="1">
+      <c r="F150">
+        <f t="shared" si="4"/>
+        <v>28.388888888888886</v>
+      </c>
+      <c r="G150" s="1">
         <v>83.1</v>
       </c>
-      <c r="G150" s="1">
+      <c r="H150" s="1">
+        <f t="shared" si="5"/>
+        <v>57.911999999999992</v>
+      </c>
+      <c r="I150" s="1">
         <v>2.2799999999999998</v>
       </c>
     </row>
-    <row r="151" spans="1:13">
+    <row r="151" spans="1:15">
       <c r="A151" t="s">
         <v>19</v>
       </c>
@@ -4070,14 +5221,22 @@
       <c r="E151">
         <v>201506</v>
       </c>
-      <c r="F151" s="1">
+      <c r="F151">
+        <f t="shared" si="4"/>
+        <v>28.833333333333332</v>
+      </c>
+      <c r="G151" s="1">
         <v>83.9</v>
       </c>
-      <c r="G151" s="1">
+      <c r="H151" s="1">
+        <f t="shared" si="5"/>
+        <v>53.593999999999994</v>
+      </c>
+      <c r="I151" s="1">
         <v>2.11</v>
       </c>
     </row>
-    <row r="152" spans="1:13">
+    <row r="152" spans="1:15">
       <c r="A152" t="s">
         <v>19</v>
       </c>
@@ -4093,14 +5252,22 @@
       <c r="E152">
         <v>201507</v>
       </c>
-      <c r="F152" s="1">
+      <c r="F152">
+        <f t="shared" si="4"/>
+        <v>28.722222222222221</v>
+      </c>
+      <c r="G152" s="1">
         <v>83.7</v>
       </c>
-      <c r="G152" s="1">
+      <c r="H152" s="1">
+        <f t="shared" si="5"/>
+        <v>40.893999999999998</v>
+      </c>
+      <c r="I152" s="1">
         <v>1.61</v>
       </c>
     </row>
-    <row r="153" spans="1:13">
+    <row r="153" spans="1:15">
       <c r="A153" t="s">
         <v>19</v>
       </c>
@@ -4116,14 +5283,22 @@
       <c r="E153">
         <v>201508</v>
       </c>
-      <c r="F153" s="1">
+      <c r="F153">
+        <f t="shared" si="4"/>
+        <v>28.444444444444443</v>
+      </c>
+      <c r="G153" s="1">
         <v>83.2</v>
       </c>
-      <c r="G153" s="1">
+      <c r="H153" s="1">
+        <f t="shared" si="5"/>
+        <v>150.62199999999999</v>
+      </c>
+      <c r="I153" s="1">
         <v>5.93</v>
       </c>
     </row>
-    <row r="154" spans="1:13">
+    <row r="154" spans="1:15">
       <c r="A154" t="s">
         <v>19</v>
       </c>
@@ -4139,14 +5314,22 @@
       <c r="E154">
         <v>201509</v>
       </c>
-      <c r="F154" s="1">
+      <c r="F154">
+        <f t="shared" si="4"/>
+        <v>29.055555555555557</v>
+      </c>
+      <c r="G154" s="1">
         <v>84.3</v>
       </c>
-      <c r="G154" s="1">
+      <c r="H154" s="1">
+        <f t="shared" si="5"/>
+        <v>109.21999999999998</v>
+      </c>
+      <c r="I154" s="1">
         <v>4.3</v>
       </c>
     </row>
-    <row r="155" spans="1:13">
+    <row r="155" spans="1:15">
       <c r="A155" t="s">
         <v>19</v>
       </c>
@@ -4162,14 +5345,22 @@
       <c r="E155">
         <v>201510</v>
       </c>
-      <c r="F155" s="1">
+      <c r="F155">
+        <f t="shared" si="4"/>
+        <v>29.222222222222221</v>
+      </c>
+      <c r="G155" s="1">
         <v>84.6</v>
       </c>
-      <c r="G155" s="1">
+      <c r="H155" s="1">
+        <f t="shared" si="5"/>
+        <v>44.957999999999998</v>
+      </c>
+      <c r="I155" s="1">
         <v>1.77</v>
       </c>
     </row>
-    <row r="156" spans="1:13">
+    <row r="156" spans="1:15">
       <c r="A156" t="s">
         <v>19</v>
       </c>
@@ -4185,14 +5376,22 @@
       <c r="E156">
         <v>201511</v>
       </c>
-      <c r="F156" s="1">
+      <c r="F156">
+        <f t="shared" si="4"/>
+        <v>27.333333333333332</v>
+      </c>
+      <c r="G156" s="1">
         <v>81.2</v>
       </c>
-      <c r="G156" s="1">
+      <c r="H156" s="1">
+        <f t="shared" si="5"/>
+        <v>221.488</v>
+      </c>
+      <c r="I156" s="1">
         <v>8.7200000000000006</v>
       </c>
     </row>
-    <row r="157" spans="1:13">
+    <row r="157" spans="1:15">
       <c r="A157" t="s">
         <v>19</v>
       </c>
@@ -4208,14 +5407,22 @@
       <c r="E157">
         <v>201512</v>
       </c>
-      <c r="F157" s="1">
+      <c r="F157">
+        <f t="shared" si="4"/>
+        <v>26.666666666666668</v>
+      </c>
+      <c r="G157" s="1">
         <v>80</v>
       </c>
-      <c r="G157" s="1">
+      <c r="H157" s="1">
+        <f t="shared" si="5"/>
+        <v>88.138000000000005</v>
+      </c>
+      <c r="I157" s="1">
         <v>3.47</v>
       </c>
     </row>
-    <row r="158" spans="1:13">
+    <row r="158" spans="1:15">
       <c r="A158" t="s">
         <v>20</v>
       </c>
@@ -4231,14 +5438,22 @@
       <c r="E158">
         <v>201501</v>
       </c>
-      <c r="F158" s="1">
+      <c r="F158">
+        <f t="shared" si="4"/>
+        <v>25.611111111111107</v>
+      </c>
+      <c r="G158" s="1">
         <v>78.099999999999994</v>
       </c>
-      <c r="G158" s="1">
+      <c r="H158" s="1">
+        <f t="shared" si="5"/>
+        <v>126.23799999999999</v>
+      </c>
+      <c r="I158" s="1">
         <v>4.97</v>
       </c>
     </row>
-    <row r="159" spans="1:13">
+    <row r="159" spans="1:15">
       <c r="A159" t="s">
         <v>20</v>
       </c>
@@ -4254,14 +5469,22 @@
       <c r="E159">
         <v>201502</v>
       </c>
-      <c r="F159" s="1">
+      <c r="F159">
+        <f t="shared" si="4"/>
+        <v>25.777777777777782</v>
+      </c>
+      <c r="G159" s="1">
         <v>78.400000000000006</v>
       </c>
-      <c r="G159" s="1">
+      <c r="H159" s="1">
+        <f t="shared" si="5"/>
+        <v>79.756</v>
+      </c>
+      <c r="I159" s="1">
         <v>3.14</v>
       </c>
     </row>
-    <row r="160" spans="1:13">
+    <row r="160" spans="1:15">
       <c r="A160" t="s">
         <v>20</v>
       </c>
@@ -4277,19 +5500,27 @@
       <c r="E160">
         <v>201503</v>
       </c>
-      <c r="F160" s="1">
+      <c r="F160">
+        <f t="shared" si="4"/>
+        <v>25.388888888888889</v>
+      </c>
+      <c r="G160" s="1">
         <v>77.7</v>
       </c>
-      <c r="G160" s="1">
+      <c r="H160" s="1">
+        <f t="shared" si="5"/>
+        <v>64.515999999999991</v>
+      </c>
+      <c r="I160" s="1">
         <v>2.54</v>
       </c>
-      <c r="H160" s="1"/>
-      <c r="I160" s="1"/>
       <c r="J160" s="1"/>
       <c r="K160" s="1"/>
       <c r="L160" s="1"/>
-    </row>
-    <row r="161" spans="1:12">
+      <c r="M160" s="1"/>
+      <c r="N160" s="1"/>
+    </row>
+    <row r="161" spans="1:14">
       <c r="A161" t="s">
         <v>20</v>
       </c>
@@ -4305,19 +5536,27 @@
       <c r="E161">
         <v>201504</v>
       </c>
-      <c r="F161" s="1">
+      <c r="F161">
+        <f t="shared" si="4"/>
+        <v>26.888888888888893</v>
+      </c>
+      <c r="G161" s="1">
         <v>80.400000000000006</v>
       </c>
-      <c r="G161" s="1">
+      <c r="H161" s="1">
+        <f t="shared" si="5"/>
+        <v>40.893999999999998</v>
+      </c>
+      <c r="I161" s="1">
         <v>1.61</v>
       </c>
-      <c r="H161" s="1"/>
-      <c r="I161" s="1"/>
       <c r="J161" s="1"/>
       <c r="K161" s="1"/>
       <c r="L161" s="1"/>
-    </row>
-    <row r="162" spans="1:12">
+      <c r="M161" s="1"/>
+      <c r="N161" s="1"/>
+    </row>
+    <row r="162" spans="1:14">
       <c r="A162" t="s">
         <v>20</v>
       </c>
@@ -4333,14 +5572,22 @@
       <c r="E162">
         <v>201505</v>
       </c>
-      <c r="F162" s="1">
+      <c r="F162">
+        <f t="shared" si="4"/>
+        <v>27.944444444444443</v>
+      </c>
+      <c r="G162" s="1">
         <v>82.3</v>
       </c>
-      <c r="G162" s="1">
+      <c r="H162" s="1">
+        <f t="shared" si="5"/>
+        <v>67.817999999999998</v>
+      </c>
+      <c r="I162" s="1">
         <v>2.67</v>
       </c>
     </row>
-    <row r="163" spans="1:12">
+    <row r="163" spans="1:14">
       <c r="A163" t="s">
         <v>20</v>
       </c>
@@ -4356,14 +5603,22 @@
       <c r="E163">
         <v>201506</v>
       </c>
-      <c r="F163" s="1">
+      <c r="F163">
+        <f t="shared" si="4"/>
+        <v>28.611111111111111</v>
+      </c>
+      <c r="G163" s="1">
         <v>83.5</v>
       </c>
-      <c r="G163" s="1">
+      <c r="H163" s="1">
+        <f t="shared" si="5"/>
+        <v>57.403999999999989</v>
+      </c>
+      <c r="I163" s="1">
         <v>2.2599999999999998</v>
       </c>
     </row>
-    <row r="164" spans="1:12">
+    <row r="164" spans="1:14">
       <c r="A164" t="s">
         <v>20</v>
       </c>
@@ -4379,14 +5634,22 @@
       <c r="E164">
         <v>201507</v>
       </c>
-      <c r="F164" s="1">
+      <c r="F164">
+        <f t="shared" si="4"/>
+        <v>28.666666666666668</v>
+      </c>
+      <c r="G164" s="1">
         <v>83.6</v>
       </c>
-      <c r="G164" s="1">
+      <c r="H164" s="1">
+        <f t="shared" si="5"/>
+        <v>51.815999999999995</v>
+      </c>
+      <c r="I164" s="1">
         <v>2.04</v>
       </c>
     </row>
-    <row r="165" spans="1:12">
+    <row r="165" spans="1:14">
       <c r="A165" t="s">
         <v>20</v>
       </c>
@@ -4402,14 +5665,22 @@
       <c r="E165">
         <v>201508</v>
       </c>
-      <c r="F165" s="1">
+      <c r="F165">
+        <f t="shared" si="4"/>
+        <v>28.666666666666668</v>
+      </c>
+      <c r="G165" s="1">
         <v>83.6</v>
       </c>
-      <c r="G165" s="1">
+      <c r="H165" s="1">
+        <f t="shared" si="5"/>
+        <v>167.89400000000001</v>
+      </c>
+      <c r="I165" s="1">
         <v>6.61</v>
       </c>
     </row>
-    <row r="166" spans="1:12">
+    <row r="166" spans="1:14">
       <c r="A166" t="s">
         <v>20</v>
       </c>
@@ -4425,14 +5696,22 @@
       <c r="E166">
         <v>201509</v>
       </c>
-      <c r="F166" s="1">
+      <c r="F166">
+        <f t="shared" si="4"/>
+        <v>28.555555555555557</v>
+      </c>
+      <c r="G166" s="1">
         <v>83.4</v>
       </c>
-      <c r="G166" s="1">
+      <c r="H166" s="1">
+        <f t="shared" si="5"/>
+        <v>106.934</v>
+      </c>
+      <c r="I166" s="1">
         <v>4.21</v>
       </c>
     </row>
-    <row r="167" spans="1:12">
+    <row r="167" spans="1:14">
       <c r="A167" t="s">
         <v>20</v>
       </c>
@@ -4448,14 +5727,22 @@
       <c r="E167">
         <v>201510</v>
       </c>
-      <c r="F167" s="1">
+      <c r="F167">
+        <f t="shared" si="4"/>
+        <v>28.722222222222221</v>
+      </c>
+      <c r="G167" s="1">
         <v>83.7</v>
       </c>
-      <c r="G167" s="1">
+      <c r="H167" s="1">
+        <f t="shared" si="5"/>
+        <v>81.025999999999996</v>
+      </c>
+      <c r="I167" s="1">
         <v>3.19</v>
       </c>
     </row>
-    <row r="168" spans="1:12">
+    <row r="168" spans="1:14">
       <c r="A168" t="s">
         <v>20</v>
       </c>
@@ -4471,14 +5758,22 @@
       <c r="E168">
         <v>201511</v>
       </c>
-      <c r="F168" s="1">
+      <c r="F168">
+        <f t="shared" si="4"/>
+        <v>27.055555555555557</v>
+      </c>
+      <c r="G168" s="1">
         <v>80.7</v>
       </c>
-      <c r="G168" s="1">
+      <c r="H168" s="1">
+        <f t="shared" si="5"/>
+        <v>250.44399999999996</v>
+      </c>
+      <c r="I168" s="1">
         <v>9.86</v>
       </c>
     </row>
-    <row r="169" spans="1:12">
+    <row r="169" spans="1:14">
       <c r="A169" t="s">
         <v>20</v>
       </c>
@@ -4494,14 +5789,22 @@
       <c r="E169">
         <v>201512</v>
       </c>
-      <c r="F169" s="1">
+      <c r="F169">
+        <f t="shared" si="4"/>
+        <v>26.333333333333336</v>
+      </c>
+      <c r="G169" s="1">
         <v>79.400000000000006</v>
       </c>
-      <c r="G169" s="1">
+      <c r="H169" s="1">
+        <f t="shared" si="5"/>
+        <v>103.378</v>
+      </c>
+      <c r="I169" s="1">
         <v>4.07</v>
       </c>
     </row>
-    <row r="170" spans="1:12">
+    <row r="170" spans="1:14">
       <c r="A170" t="s">
         <v>21</v>
       </c>
@@ -4517,14 +5820,21 @@
       <c r="E170">
         <v>201501</v>
       </c>
-      <c r="F170" s="1">
+      <c r="F170">
+        <f t="shared" si="4"/>
+        <v>25.611111111111107</v>
+      </c>
+      <c r="G170" s="1">
         <v>78.099999999999994</v>
       </c>
-      <c r="G170" s="1">
-        <v>-9999</v>
-      </c>
-    </row>
-    <row r="171" spans="1:12">
+      <c r="H170" s="1">
+        <v>-9999</v>
+      </c>
+      <c r="I170" s="1">
+        <v>-9999</v>
+      </c>
+    </row>
+    <row r="171" spans="1:14">
       <c r="A171" t="s">
         <v>21</v>
       </c>
@@ -4540,14 +5850,22 @@
       <c r="E171">
         <v>201502</v>
       </c>
-      <c r="F171" s="1">
+      <c r="F171">
+        <f t="shared" si="4"/>
+        <v>25.777777777777782</v>
+      </c>
+      <c r="G171" s="1">
         <v>78.400000000000006</v>
       </c>
-      <c r="G171" s="1">
+      <c r="H171" s="1">
+        <f t="shared" si="5"/>
+        <v>110.23599999999999</v>
+      </c>
+      <c r="I171" s="1">
         <v>4.34</v>
       </c>
     </row>
-    <row r="172" spans="1:12">
+    <row r="172" spans="1:14">
       <c r="A172" t="s">
         <v>21</v>
       </c>
@@ -4563,14 +5881,21 @@
       <c r="E172">
         <v>201503</v>
       </c>
-      <c r="F172" s="1">
+      <c r="F172">
+        <f t="shared" si="4"/>
+        <v>25.611111111111107</v>
+      </c>
+      <c r="G172" s="1">
         <v>78.099999999999994</v>
       </c>
-      <c r="G172" s="1">
-        <v>-9999</v>
-      </c>
-    </row>
-    <row r="173" spans="1:12">
+      <c r="H172" s="1">
+        <v>-9999</v>
+      </c>
+      <c r="I172" s="1">
+        <v>-9999</v>
+      </c>
+    </row>
+    <row r="173" spans="1:14">
       <c r="A173" t="s">
         <v>21</v>
       </c>
@@ -4586,14 +5911,22 @@
       <c r="E173">
         <v>201504</v>
       </c>
-      <c r="F173" s="1">
+      <c r="F173">
+        <f t="shared" si="4"/>
+        <v>26.999999999999996</v>
+      </c>
+      <c r="G173" s="1">
         <v>80.599999999999994</v>
       </c>
-      <c r="G173" s="1">
+      <c r="H173" s="1">
+        <f t="shared" si="5"/>
+        <v>59.69</v>
+      </c>
+      <c r="I173" s="1">
         <v>2.35</v>
       </c>
     </row>
-    <row r="174" spans="1:12">
+    <row r="174" spans="1:14">
       <c r="A174" t="s">
         <v>21</v>
       </c>
@@ -4609,19 +5942,27 @@
       <c r="E174">
         <v>201505</v>
       </c>
-      <c r="F174" s="1">
+      <c r="F174">
+        <f t="shared" si="4"/>
+        <v>28.333333333333332</v>
+      </c>
+      <c r="G174" s="1">
         <v>83</v>
       </c>
-      <c r="G174" s="1">
+      <c r="H174" s="1">
+        <f t="shared" si="5"/>
+        <v>102.10799999999999</v>
+      </c>
+      <c r="I174" s="1">
         <v>4.0199999999999996</v>
       </c>
-      <c r="H174" s="1"/>
-      <c r="I174" s="1"/>
       <c r="J174" s="1"/>
       <c r="K174" s="1"/>
       <c r="L174" s="1"/>
-    </row>
-    <row r="175" spans="1:12">
+      <c r="M174" s="1"/>
+      <c r="N174" s="1"/>
+    </row>
+    <row r="175" spans="1:14">
       <c r="A175" t="s">
         <v>21</v>
       </c>
@@ -4637,14 +5978,22 @@
       <c r="E175">
         <v>201506</v>
       </c>
-      <c r="F175" s="1">
+      <c r="F175">
+        <f t="shared" si="4"/>
+        <v>29.055555555555557</v>
+      </c>
+      <c r="G175" s="1">
         <v>84.3</v>
       </c>
-      <c r="G175" s="1">
+      <c r="H175" s="1">
+        <f t="shared" si="5"/>
+        <v>25.654</v>
+      </c>
+      <c r="I175" s="1">
         <v>1.01</v>
       </c>
     </row>
-    <row r="176" spans="1:12">
+    <row r="176" spans="1:14">
       <c r="A176" t="s">
         <v>21</v>
       </c>
@@ -4660,14 +6009,21 @@
       <c r="E176">
         <v>201507</v>
       </c>
-      <c r="F176" s="1">
+      <c r="F176">
+        <f t="shared" si="4"/>
+        <v>28.888888888888889</v>
+      </c>
+      <c r="G176" s="1">
         <v>84</v>
       </c>
-      <c r="G176" s="1">
-        <v>-9999</v>
-      </c>
-    </row>
-    <row r="177" spans="1:12">
+      <c r="H176" s="1">
+        <v>-9999</v>
+      </c>
+      <c r="I176" s="1">
+        <v>-9999</v>
+      </c>
+    </row>
+    <row r="177" spans="1:14">
       <c r="A177" t="s">
         <v>21</v>
       </c>
@@ -4683,14 +6039,22 @@
       <c r="E177">
         <v>201508</v>
       </c>
-      <c r="F177" s="1">
+      <c r="F177">
+        <f t="shared" si="4"/>
+        <v>28.777777777777779</v>
+      </c>
+      <c r="G177" s="1">
         <v>83.8</v>
       </c>
-      <c r="G177" s="1">
+      <c r="H177" s="1">
+        <f t="shared" si="5"/>
+        <v>142.74799999999999</v>
+      </c>
+      <c r="I177" s="1">
         <v>5.62</v>
       </c>
     </row>
-    <row r="178" spans="1:12">
+    <row r="178" spans="1:14">
       <c r="A178" t="s">
         <v>21</v>
       </c>
@@ -4706,14 +6070,21 @@
       <c r="E178">
         <v>201509</v>
       </c>
-      <c r="F178" s="1">
+      <c r="F178">
+        <f t="shared" si="4"/>
+        <v>28.944444444444443</v>
+      </c>
+      <c r="G178" s="1">
         <v>84.1</v>
       </c>
-      <c r="G178" s="1">
-        <v>-9999</v>
-      </c>
-    </row>
-    <row r="179" spans="1:12">
+      <c r="H178" s="1">
+        <v>-9999</v>
+      </c>
+      <c r="I178" s="1">
+        <v>-9999</v>
+      </c>
+    </row>
+    <row r="179" spans="1:14">
       <c r="A179" t="s">
         <v>21</v>
       </c>
@@ -4729,14 +6100,21 @@
       <c r="E179">
         <v>201510</v>
       </c>
-      <c r="F179" s="1">
+      <c r="F179">
+        <f t="shared" si="4"/>
+        <v>28.833333333333332</v>
+      </c>
+      <c r="G179" s="1">
         <v>83.9</v>
       </c>
-      <c r="G179" s="1">
-        <v>-9999</v>
-      </c>
-    </row>
-    <row r="180" spans="1:12">
+      <c r="H179" s="1">
+        <v>-9999</v>
+      </c>
+      <c r="I179" s="1">
+        <v>-9999</v>
+      </c>
+    </row>
+    <row r="180" spans="1:14">
       <c r="A180" t="s">
         <v>21</v>
       </c>
@@ -4752,19 +6130,25 @@
       <c r="E180">
         <v>201511</v>
       </c>
-      <c r="F180" s="1">
+      <c r="F180">
         <v>-9999</v>
       </c>
       <c r="G180" s="1">
         <v>-9999</v>
       </c>
-      <c r="H180" s="1"/>
-      <c r="I180" s="1"/>
+      <c r="H180" s="1">
+        <v>-9999</v>
+      </c>
+      <c r="I180" s="1">
+        <v>-9999</v>
+      </c>
       <c r="J180" s="1"/>
       <c r="K180" s="1"/>
       <c r="L180" s="1"/>
-    </row>
-    <row r="181" spans="1:12">
+      <c r="M180" s="1"/>
+      <c r="N180" s="1"/>
+    </row>
+    <row r="181" spans="1:14">
       <c r="A181" t="s">
         <v>21</v>
       </c>
@@ -4780,78 +6164,97 @@
       <c r="E181">
         <v>201512</v>
       </c>
-      <c r="F181" s="1">
+      <c r="F181">
+        <f t="shared" si="4"/>
+        <v>26.277777777777779</v>
+      </c>
+      <c r="G181" s="1">
         <v>79.3</v>
       </c>
-      <c r="G181" s="1">
-        <v>-9999</v>
-      </c>
-    </row>
-    <row r="182" spans="1:12">
-      <c r="F182" s="1"/>
+      <c r="H181" s="1">
+        <v>-9999</v>
+      </c>
+      <c r="I181" s="1">
+        <v>-9999</v>
+      </c>
+    </row>
+    <row r="182" spans="1:14">
       <c r="G182" s="1"/>
-    </row>
-    <row r="183" spans="1:12">
+      <c r="H182" s="1"/>
+      <c r="I182" s="1"/>
+    </row>
+    <row r="183" spans="1:14">
       <c r="B183" s="1"/>
       <c r="C183" s="1"/>
       <c r="D183" s="1"/>
-      <c r="F183" s="1"/>
       <c r="G183" s="1"/>
       <c r="H183" s="1"/>
       <c r="I183" s="1"/>
       <c r="J183" s="1"/>
       <c r="K183" s="1"/>
       <c r="L183" s="1"/>
-    </row>
-    <row r="184" spans="1:12">
+      <c r="M183" s="1"/>
+      <c r="N183" s="1"/>
+    </row>
+    <row r="184" spans="1:14">
       <c r="B184" s="1"/>
       <c r="C184" s="1"/>
       <c r="D184" s="1"/>
-      <c r="F184" s="1"/>
       <c r="G184" s="1"/>
       <c r="H184" s="1"/>
       <c r="I184" s="1"/>
       <c r="J184" s="1"/>
       <c r="K184" s="1"/>
       <c r="L184" s="1"/>
-    </row>
-    <row r="185" spans="1:12">
-      <c r="F185" s="1"/>
+      <c r="M184" s="1"/>
+      <c r="N184" s="1"/>
+    </row>
+    <row r="185" spans="1:14">
       <c r="G185" s="1"/>
-    </row>
-    <row r="186" spans="1:12">
-      <c r="F186" s="1"/>
+      <c r="H185" s="1"/>
+      <c r="I185" s="1"/>
+    </row>
+    <row r="186" spans="1:14">
       <c r="G186" s="1"/>
-    </row>
-    <row r="187" spans="1:12">
-      <c r="F187" s="1"/>
+      <c r="H186" s="1"/>
+      <c r="I186" s="1"/>
+    </row>
+    <row r="187" spans="1:14">
       <c r="G187" s="1"/>
-    </row>
-    <row r="188" spans="1:12">
-      <c r="F188" s="1"/>
+      <c r="H187" s="1"/>
+      <c r="I187" s="1"/>
+    </row>
+    <row r="188" spans="1:14">
       <c r="G188" s="1"/>
-    </row>
-    <row r="189" spans="1:12">
-      <c r="F189" s="1"/>
+      <c r="H188" s="1"/>
+      <c r="I188" s="1"/>
+    </row>
+    <row r="189" spans="1:14">
       <c r="G189" s="1"/>
-    </row>
-    <row r="190" spans="1:12">
-      <c r="F190" s="1"/>
+      <c r="H189" s="1"/>
+      <c r="I189" s="1"/>
+    </row>
+    <row r="190" spans="1:14">
       <c r="G190" s="1"/>
-    </row>
-    <row r="191" spans="1:12">
-      <c r="F191" s="1"/>
+      <c r="H190" s="1"/>
+      <c r="I190" s="1"/>
+    </row>
+    <row r="191" spans="1:14">
       <c r="G191" s="1"/>
-    </row>
-    <row r="192" spans="1:12">
-      <c r="F192" s="1"/>
+      <c r="H191" s="1"/>
+      <c r="I191" s="1"/>
+    </row>
+    <row r="192" spans="1:14">
       <c r="G192" s="1"/>
-    </row>
-    <row r="193" spans="1:12">
-      <c r="F193" s="1"/>
+      <c r="H192" s="1"/>
+      <c r="I192" s="1"/>
+    </row>
+    <row r="193" spans="1:14">
       <c r="G193" s="1"/>
-    </row>
-    <row r="195" spans="1:12">
+      <c r="H193" s="1"/>
+      <c r="I193" s="1"/>
+    </row>
+    <row r="195" spans="1:14">
       <c r="A195" s="1"/>
       <c r="B195" s="1"/>
       <c r="C195" s="1"/>
@@ -4864,8 +6267,10 @@
       <c r="J195" s="1"/>
       <c r="K195" s="1"/>
       <c r="L195" s="1"/>
-    </row>
-    <row r="196" spans="1:12">
+      <c r="M195" s="1"/>
+      <c r="N195" s="1"/>
+    </row>
+    <row r="196" spans="1:14">
       <c r="A196" s="1"/>
       <c r="B196" s="1"/>
       <c r="C196" s="1"/>
@@ -4878,10 +6283,12 @@
       <c r="J196" s="1"/>
       <c r="K196" s="1"/>
       <c r="L196" s="1"/>
+      <c r="M196" s="1"/>
+      <c r="N196" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -4891,12 +6298,12 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
@@ -4908,12 +6315,12 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>

</xml_diff>